<commit_message>
update LCA for the system
</commit_message>
<xml_diff>
--- a/exposan/htl/data/impact_items.xlsx
+++ b/exposan/htl/data/impact_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiananfeng/Desktop/PhD CEE/coding/Cloned packages/EXPOsan/exposan/htl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6DCC63-8CB9-EC46-9E13-F264DDD10B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8FA609-58FA-3947-A20F-6F7B7606D9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12540" yWindow="29300" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="11240" yWindow="4660" windowWidth="28800" windowHeight="17500" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -192,9 +192,6 @@
     <t>RoW</t>
   </si>
   <si>
-    <t>natural gas liquids production</t>
-  </si>
-  <si>
     <t>liquid</t>
   </si>
   <si>
@@ -282,18 +279,12 @@
     <t>market for cooling energy</t>
   </si>
   <si>
-    <t>natural gas, burned in micro gas turbine</t>
-  </si>
-  <si>
     <t>diluted to 5% using deionized water</t>
   </si>
   <si>
     <t>Rhodium</t>
   </si>
   <si>
-    <t>liquid/if used, account for  CO2 emission here, add to GWP only, MW of natural gas is 19 (1 C): https://www.engineeringtoolbox.com/molecular-weight-gas-vapor-d_1156.html (accessed 12-2-2022)</t>
-  </si>
-  <si>
     <t>ea</t>
   </si>
   <si>
@@ -364,6 +355,15 @@
   </si>
   <si>
     <t>HTHC_catalyst</t>
+  </si>
+  <si>
+    <t>Diesel_for_calc</t>
+  </si>
+  <si>
+    <t>market for natural gas, burned in gas motor, for storage</t>
+  </si>
+  <si>
+    <t>includle burning emission, 1 kg natural gas = 24.624 MJ (see Ecoinvent: market for natural gas liquids)</t>
   </si>
 </sst>
 </file>
@@ -404,12 +404,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -424,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -435,6 +441,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66379A7A-E84B-1346-816F-577916F7D6A6}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -784,7 +792,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -818,13 +826,13 @@
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>33</v>
@@ -833,13 +841,13 @@
     </row>
     <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>33</v>
@@ -848,7 +856,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
@@ -862,7 +870,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
@@ -876,7 +884,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -899,7 +907,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>33</v>
@@ -913,23 +921,23 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -989,7 +997,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>33</v>
@@ -997,24 +1005,24 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
@@ -1028,47 +1036,47 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>33</v>
@@ -1076,39 +1084,39 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>48</v>
@@ -1116,13 +1124,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>48</v>
@@ -1130,13 +1138,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>48</v>
@@ -1144,13 +1152,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>33</v>
@@ -1158,13 +1166,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>33</v>
@@ -1172,13 +1180,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>33</v>
@@ -1186,7 +1194,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>8</v>
@@ -1203,13 +1211,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>33</v>
@@ -1217,13 +1225,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>33</v>
@@ -1231,13 +1239,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>33</v>
@@ -1245,13 +1253,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>48</v>
@@ -1262,30 +1270,30 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>33</v>
@@ -1293,27 +1301,27 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>48</v>
@@ -1321,19 +1329,19 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1349,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32918E97-33AC-4743-867D-87B08CF8DB3F}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1388,7 +1396,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>28</v>
@@ -1440,7 +1448,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>28</v>
@@ -1465,7 +1473,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>28</v>
@@ -1490,7 +1498,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>28</v>
@@ -1515,7 +1523,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>28</v>
@@ -1540,7 +1548,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>28</v>
@@ -1741,7 +1749,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>28</v>
@@ -1767,7 +1775,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>28</v>
@@ -1792,21 +1800,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="2">
-        <v>4.8979000000000004E-4</v>
+      <c r="C18" s="9">
+        <f>C36*24.624</f>
+        <v>3.50916624E-4</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>4.4081100000000005E-4</v>
+        <v>3.1582496160000002E-4</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>5.3876900000000014E-4</v>
+        <v>3.8600828640000004E-4</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>1</v>
@@ -1817,7 +1826,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>28</v>
@@ -1842,21 +1851,21 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="2">
-        <v>1.1096000000000001E-3</v>
+        <v>-1.1096000000000001E-3</v>
       </c>
       <c r="D20" s="2">
         <f>C20*0.9</f>
-        <v>9.9864000000000007E-4</v>
+        <v>-9.9864000000000007E-4</v>
       </c>
       <c r="E20" s="2">
         <f>C20*1.1</f>
-        <v>1.2205600000000001E-3</v>
+        <v>-1.2205600000000001E-3</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>1</v>
@@ -1867,22 +1876,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C21" s="2">
         <f>0.147*C37+0.1222*C35+87.3/3600*C38+2.3704*C37+0.312*C36+(1000-1000*7.8/100/101.07*207.43)/1000*C31+0.9454*C24+1000*7.8/100/1000*C32/35335*2665+1000*7.8/100/101.07*(207.43-101.07)/1000*C33+0.487*1000*7.8/100/101.07*207.43/1000*C38+2.59/1000*C34</f>
-        <v>3.5171845258375174</v>
+        <v>3.5171796523975174</v>
       </c>
       <c r="D21" s="2">
         <f>C21*0.9</f>
-        <v>3.1654660732537656</v>
+        <v>3.1654616871577659</v>
       </c>
       <c r="E21" s="2">
         <f>C21*1.1</f>
-        <v>3.8689029784212696</v>
+        <v>3.8688976176372694</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>1</v>
@@ -1893,22 +1902,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="2">
         <f>0.4168*C36+3.358*C35+0.206*C37+1.6569*C37+0.4856*C36+0.0149*C38+1.2669*C36+0.7722*C23+0.6177*C24+0.0349*C25+0.136*C26+0.0834*C27+0.0973*C28+0.0088*C29+1.301*C30</f>
-        <v>2.0809293373641003E-2</v>
+        <v>2.0775408907641003E-2</v>
       </c>
       <c r="D22" s="2">
         <f>C22*0.9</f>
-        <v>1.8728364036276902E-2</v>
+        <v>1.8697868016876902E-2</v>
       </c>
       <c r="E22" s="2">
         <f>C22*1.1</f>
-        <v>2.2890222711005104E-2</v>
+        <v>2.2852949798405103E-2</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>1</v>
@@ -1919,7 +1928,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>28</v>
@@ -1944,7 +1953,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>28</v>
@@ -1969,7 +1978,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>28</v>
@@ -1994,7 +2003,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>28</v>
@@ -2019,7 +2028,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>28</v>
@@ -2044,7 +2053,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>28</v>
@@ -2069,7 +2078,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>28</v>
@@ -2094,7 +2103,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>28</v>
@@ -2119,7 +2128,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>28</v>
@@ -2144,7 +2153,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>28</v>
@@ -2169,7 +2178,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>28</v>
@@ -2194,7 +2203,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>28</v>
@@ -2219,7 +2228,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>28</v>
@@ -2244,21 +2253,21 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C36" s="6">
-        <v>2.9870999999999999E-5</v>
+        <v>1.4251E-5</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" si="8"/>
-        <v>2.6883899999999999E-5</v>
+        <v>1.28259E-5</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="9"/>
-        <v>3.2858100000000003E-5</v>
+        <v>1.5676100000000001E-5</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>1</v>
@@ -2269,7 +2278,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>28</v>
@@ -2294,7 +2303,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>28</v>
@@ -2328,8 +2337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B44E52-5A7F-8142-BD9E-CE1C29D2C0B8}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A5" zoomScale="106" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2367,7 +2376,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>21</v>
@@ -2419,7 +2428,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>21</v>
@@ -2444,7 +2453,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>21</v>
@@ -2469,7 +2478,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>21</v>
@@ -2494,7 +2503,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>21</v>
@@ -2519,7 +2528,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>21</v>
@@ -2720,7 +2729,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>21</v>
@@ -2746,7 +2755,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>21</v>
@@ -2771,21 +2780,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="2">
-        <v>0.1032</v>
+        <f>C36*24.624</f>
+        <v>8.3822558399999997E-2</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>9.2880000000000004E-2</v>
+        <v>7.5440302560000005E-2</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>0.11352000000000001</v>
+        <v>9.2204814240000002E-2</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>1</v>
@@ -2796,7 +2806,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>21</v>
@@ -2821,21 +2831,21 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="2">
-        <v>0.25163999999999997</v>
+        <v>-0.25163999999999997</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" ref="D20" si="8">C20*0.9</f>
-        <v>0.22647599999999998</v>
+        <v>-0.22647599999999998</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" ref="E20" si="9">C20*1.1</f>
-        <v>0.27680399999999999</v>
+        <v>-0.27680399999999999</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>1</v>
@@ -2846,22 +2856,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="2">
         <f>0.147*C37+0.1222*C35+87.3/3600*C38+2.3704*C37+0.312*C36+(1000-1000*7.8/100/101.07*207.43)/1000*C31+0.9454*C24+1000*7.8/100/1000*C32/35335*2665+1000*7.8/100/101.07*(207.43-101.07)/1000*C33+0.487*1000*7.8/100/101.07*207.43/1000*C38+2.59/1000*C34</f>
-        <v>991.65441961282067</v>
+        <v>991.65279880402068</v>
       </c>
       <c r="D21" s="2">
         <f>C21*0.9</f>
-        <v>892.48897765153868</v>
+        <v>892.48751892361861</v>
       </c>
       <c r="E21" s="2">
         <f>C21*1.1</f>
-        <v>1090.8198615741028</v>
+        <v>1090.8180786844227</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>1</v>
@@ -2872,22 +2882,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="2">
         <f>0.4168*C36+3.358*C35+0.206*C37+1.6569*C37+0.4856*C36+0.0149*C38+1.2669*C36+0.7722*C23+0.6177*C24+0.0349*C25+0.136*C26+0.0834*C27+0.0973*C28+0.0088*C29+1.301*C30</f>
-        <v>4.0564012825520006</v>
+        <v>4.0451319859820005</v>
       </c>
       <c r="D22" s="2">
         <f>C22*0.9</f>
-        <v>3.6507611542968008</v>
+        <v>3.6406187873838007</v>
       </c>
       <c r="E22" s="2">
         <f>C22*1.1</f>
-        <v>4.4620414108072008</v>
+        <v>4.4496451845802012</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>1</v>
@@ -2898,7 +2908,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>21</v>
@@ -2923,7 +2933,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>21</v>
@@ -2948,7 +2958,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>21</v>
@@ -2973,7 +2983,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>21</v>
@@ -2998,7 +3008,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>21</v>
@@ -3023,7 +3033,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>21</v>
@@ -3048,7 +3058,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>21</v>
@@ -3073,7 +3083,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>21</v>
@@ -3098,7 +3108,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>21</v>
@@ -3123,7 +3133,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>21</v>
@@ -3148,7 +3158,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>21</v>
@@ -3173,7 +3183,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>21</v>
@@ -3198,7 +3208,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>21</v>
@@ -3223,21 +3233,21 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C36" s="2">
-        <v>8.5990000000000007E-3</v>
+        <v>3.4041000000000002E-3</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" si="10"/>
-        <v>7.7391000000000005E-3</v>
+        <v>3.0636900000000004E-3</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="12"/>
-        <v>9.458900000000001E-3</v>
+        <v>3.7445100000000004E-3</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>1</v>
@@ -3248,7 +3258,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>21</v>
@@ -3273,7 +3283,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>21</v>
@@ -3306,8 +3316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB3A8C1-31D1-8447-9043-3E804D12662D}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3343,7 +3353,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>22</v>
@@ -3395,7 +3405,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>22</v>
@@ -3420,7 +3430,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>22</v>
@@ -3445,7 +3455,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>22</v>
@@ -3470,7 +3480,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>22</v>
@@ -3495,7 +3505,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>22</v>
@@ -3696,7 +3706,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>22</v>
@@ -3722,7 +3732,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>22</v>
@@ -3747,21 +3757,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="2">
-        <v>0.1071</v>
+        <f>C36*24.624</f>
+        <v>6.3446198400000001E-2</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>9.6390000000000003E-2</v>
+        <v>5.7101578560000005E-2</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>0.11781000000000001</v>
+        <v>6.979081824000001E-2</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>1</v>
@@ -3772,7 +3783,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>22</v>
@@ -3797,21 +3808,21 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="2">
-        <v>0.18748000000000001</v>
+        <v>-0.18748000000000001</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" ref="D20" si="6">C20*0.9</f>
-        <v>0.16873200000000002</v>
+        <v>-0.16873200000000002</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" ref="E20" si="7">C20*1.1</f>
-        <v>0.20622800000000002</v>
+        <v>-0.20622800000000002</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>1</v>
@@ -3822,22 +3833,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="2">
         <f>0.147*C37+0.1222*C35+87.3/3600*C38+2.3704*C37+0.312*C36+(1000-1000*7.8/100/101.07*207.43)/1000*C31+0.9454*C24+1000*7.8/100/1000*C32/35335*2665+1000*7.8/100/101.07*(207.43-101.07)/1000*C33+0.487*1000*7.8/100/101.07*207.43/1000*C38+2.59/1000*C34</f>
-        <v>15371.082923819398</v>
+        <v>15371.081540660998</v>
       </c>
       <c r="D21" s="2">
         <f>C21*0.9</f>
-        <v>13833.974631437459</v>
+        <v>13833.973386594898</v>
       </c>
       <c r="E21" s="2">
         <f>C21*1.1</f>
-        <v>16908.19121620134</v>
+        <v>16908.189694727098</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>1</v>
@@ -3848,22 +3859,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="2">
         <f>0.4168*C36+3.358*C35+0.206*C37+1.6569*C37+0.4856*C36+0.0149*C38+1.2669*C36+0.7722*C23+0.6177*C24+0.0349*C25+0.136*C26+0.0834*C27+0.0973*C28+0.0088*C29+1.301*C30</f>
-        <v>50.269262735110004</v>
+        <v>50.259645794350007</v>
       </c>
       <c r="D22" s="2">
         <f>C22*0.9</f>
-        <v>45.242336461599002</v>
+        <v>45.233681214915009</v>
       </c>
       <c r="E22" s="2">
         <f>C22*1.1</f>
-        <v>55.296189008621006</v>
+        <v>55.285610373785012</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>1</v>
@@ -3874,7 +3885,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>22</v>
@@ -3899,7 +3910,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>22</v>
@@ -3924,7 +3935,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>22</v>
@@ -3949,7 +3960,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>22</v>
@@ -3974,7 +3985,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>22</v>
@@ -3999,7 +4010,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>22</v>
@@ -4024,7 +4035,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>22</v>
@@ -4049,7 +4060,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>22</v>
@@ -4074,7 +4085,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>22</v>
@@ -4099,7 +4110,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>22</v>
@@ -4124,7 +4135,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>22</v>
@@ -4149,7 +4160,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>22</v>
@@ -4174,7 +4185,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>22</v>
@@ -4199,21 +4210,21 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C36" s="2">
-        <v>7.0098000000000001E-3</v>
+        <v>2.5766000000000001E-3</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" si="8"/>
-        <v>6.3088200000000006E-3</v>
+        <v>2.3189400000000002E-3</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="9"/>
-        <v>7.7107800000000004E-3</v>
+        <v>2.8342600000000003E-3</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>1</v>
@@ -4224,7 +4235,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>22</v>
@@ -4249,7 +4260,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>22</v>
@@ -4283,7 +4294,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4320,7 +4331,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>23</v>
@@ -4372,7 +4383,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>23</v>
@@ -4397,7 +4408,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>
@@ -4422,7 +4433,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>23</v>
@@ -4447,7 +4458,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -4472,7 +4483,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>23</v>
@@ -4673,7 +4684,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
@@ -4699,7 +4710,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>23</v>
@@ -4724,21 +4735,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="6">
-        <v>7.8700000000000002E-5</v>
+        <f>C36*24.624</f>
+        <v>7.2539841599999995E-5</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>7.0829999999999998E-5</v>
+        <v>6.5285857439999992E-5</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>8.6570000000000006E-5</v>
+        <v>7.9793825759999997E-5</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>1</v>
@@ -4749,7 +4761,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
@@ -4774,21 +4786,21 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="2">
-        <v>1.0547E-3</v>
+        <v>-1.0547E-3</v>
       </c>
       <c r="D20" s="2">
         <f>C20*0.9</f>
-        <v>9.4923000000000002E-4</v>
+        <v>-9.4923000000000002E-4</v>
       </c>
       <c r="E20" s="2">
         <f>C20*1.1</f>
-        <v>1.1601700000000001E-3</v>
+        <v>-1.1601700000000001E-3</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>1</v>
@@ -4799,22 +4811,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="2">
         <f>0.147*C37+0.1222*C35+87.3/3600*C38+2.3704*C37+0.312*C36+(1000-1000*7.8/100/101.07*207.43)/1000*C31+0.9454*C24+1000*7.8/100/1000*C32/35335*2665+1000*7.8/100/101.07*(207.43-101.07)/1000*C33+0.487*1000*7.8/100/101.07*207.43/1000*C38+2.59/1000*C34</f>
-        <v>0.45019348021710359</v>
+        <v>0.45019206857310357</v>
       </c>
       <c r="D21" s="2">
         <f>C21*0.9</f>
-        <v>0.40517413219539322</v>
+        <v>0.4051728617157932</v>
       </c>
       <c r="E21" s="2">
         <f>C21*1.1</f>
-        <v>0.49521282823881402</v>
+        <v>0.49521127543041399</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>1</v>
@@ -4825,22 +4837,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="2">
         <f>0.4168*C36+3.358*C35+0.206*C37+1.6569*C37+0.4856*C36+0.0149*C38+1.2669*C36+0.7722*C23+0.6177*C24+0.0349*C25+0.136*C26+0.0834*C27+0.0973*C28+0.0088*C29+1.301*C30</f>
-        <v>5.7592737821191998E-3</v>
+        <v>5.7494587842691998E-3</v>
       </c>
       <c r="D22" s="2">
         <f>C22*0.9</f>
-        <v>5.1833464039072802E-3</v>
+        <v>5.1745129058422797E-3</v>
       </c>
       <c r="E22" s="2">
         <f>C22*1.1</f>
-        <v>6.3352011603311203E-3</v>
+        <v>6.3244046626961198E-3</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>1</v>
@@ -4851,7 +4863,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>23</v>
@@ -4876,7 +4888,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>23</v>
@@ -4901,7 +4913,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>23</v>
@@ -4926,7 +4938,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>23</v>
@@ -4951,7 +4963,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>23</v>
@@ -4976,7 +4988,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>23</v>
@@ -5001,7 +5013,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>23</v>
@@ -5026,7 +5038,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>23</v>
@@ -5051,7 +5063,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>23</v>
@@ -5076,7 +5088,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>23</v>
@@ -5101,7 +5113,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>23</v>
@@ -5126,7 +5138,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>23</v>
@@ -5151,7 +5163,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>23</v>
@@ -5176,21 +5188,21 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C36" s="6">
-        <v>7.4703999999999997E-6</v>
+        <v>2.9459E-6</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" si="10"/>
-        <v>6.7233599999999996E-6</v>
+        <v>2.6513100000000002E-6</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="11"/>
-        <v>8.2174399999999997E-6</v>
+        <v>3.2404900000000003E-6</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>1</v>
@@ -5201,7 +5213,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>23</v>
@@ -5226,7 +5238,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>23</v>
@@ -5257,10 +5269,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE2E960-887B-1E49-80AF-9619BDC224B9}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5271,7 +5283,7 @@
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -5294,9 +5306,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -5319,7 +5331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -5345,9 +5357,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>11</v>
@@ -5370,9 +5382,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>11</v>
@@ -5395,9 +5407,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -5420,9 +5432,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
@@ -5445,9 +5457,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>11</v>
@@ -5470,7 +5482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -5495,7 +5507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -5521,7 +5533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -5546,7 +5558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -5571,7 +5583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -5596,7 +5608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -5621,7 +5633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -5645,10 +5657,14 @@
       <c r="G15" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <f>1/19*44</f>
+        <v>2.3157894736842106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>11</v>
@@ -5674,7 +5690,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>11</v>
@@ -5699,22 +5715,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="2">
-        <f>0.43913+1/19*44</f>
-        <v>2.7549194736842106</v>
+      <c r="C18" s="9">
+        <f>C36*24.624</f>
+        <v>1.584234288</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>2.4794275263157894</v>
+        <v>1.4258108592000001</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>3.0304114210526318</v>
+        <v>1.7426577168000001</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>1</v>
@@ -5725,7 +5741,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>11</v>
@@ -5750,21 +5766,21 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="2">
-        <v>0.47693999999999998</v>
+        <v>-0.47693999999999998</v>
       </c>
       <c r="D20" s="2">
         <f>C20*0.9</f>
-        <v>0.42924599999999996</v>
+        <v>-0.42924599999999996</v>
       </c>
       <c r="E20" s="2">
         <f>C20*1.1</f>
-        <v>0.52463400000000004</v>
+        <v>-0.52463400000000004</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>1</v>
@@ -5775,22 +5791,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="2">
         <f>0.147*C37+0.1222*C35+87.3/3600*C38+2.3704*C37+0.312*C36+(1000-1000*7.8/100/101.07*207.43)/1000*C31+0.9454*C24+1000*7.8/100/1000*C32/35335*2665+1000*7.8/100/101.07*(207.43-101.07)/1000*C33+0.487*1000*7.8/100/101.07*207.43/1000*C38+2.59/1000*C34</f>
-        <v>484.7862509286262</v>
+        <v>484.7595334326262</v>
       </c>
       <c r="D21" s="2">
         <f>C21*0.9</f>
-        <v>436.30762583576359</v>
+        <v>436.28358008936357</v>
       </c>
       <c r="E21" s="2">
         <f>C21*1.1</f>
-        <v>533.26487602148882</v>
+        <v>533.23548677588883</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>1</v>
@@ -5801,22 +5817,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="2">
         <f>0.4168*C36+3.358*C35+0.206*C37+1.6569*C37+0.4856*C36+0.0149*C38+1.2669*C36+0.7722*C23+0.6177*C24+0.0349*C25+0.136*C26+0.0834*C27+0.0973*C28+0.0088*C29+1.301*C30</f>
-        <v>6.3758782313560003</v>
+        <v>6.1901145644560005</v>
       </c>
       <c r="D22" s="2">
         <f>C22*0.9</f>
-        <v>5.7382904082204007</v>
+        <v>5.5711031080104005</v>
       </c>
       <c r="E22" s="2">
         <f>C22*1.1</f>
-        <v>7.0134660544916008</v>
+        <v>6.8091260209016014</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>1</v>
@@ -5827,7 +5843,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>11</v>
@@ -5852,7 +5868,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>11</v>
@@ -5877,7 +5893,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>11</v>
@@ -5902,7 +5918,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>11</v>
@@ -5927,7 +5943,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>11</v>
@@ -5952,7 +5968,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>11</v>
@@ -5977,7 +5993,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>11</v>
@@ -6002,7 +6018,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>11</v>
@@ -6027,7 +6043,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>11</v>
@@ -6052,7 +6068,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>11</v>
@@ -6077,7 +6093,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>11</v>
@@ -6102,7 +6118,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>11</v>
@@ -6127,7 +6143,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>11</v>
@@ -6152,21 +6168,21 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="2">
-        <v>0.14996999999999999</v>
+        <v>6.4337000000000005E-2</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" si="8"/>
-        <v>0.13497300000000001</v>
+        <v>5.7903300000000005E-2</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="9"/>
-        <v>0.164967</v>
+        <v>7.0770700000000006E-2</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>1</v>
@@ -6177,7 +6193,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>11</v>
@@ -6202,7 +6218,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>11</v>
@@ -6236,7 +6252,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6273,7 +6289,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>24</v>
@@ -6325,7 +6341,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>24</v>
@@ -6350,7 +6366,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>24</v>
@@ -6375,7 +6391,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>24</v>
@@ -6400,7 +6416,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>24</v>
@@ -6425,7 +6441,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>24</v>
@@ -6626,7 +6642,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>24</v>
@@ -6652,7 +6668,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>24</v>
@@ -6677,21 +6693,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="6">
-        <v>2.1717999999999999E-7</v>
+      <c r="C18" s="9">
+        <f>C36*24.624</f>
+        <v>1.2338347679999998E-7</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>1.9546200000000001E-7</v>
+        <v>1.1104512911999998E-7</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>2.38898E-7</v>
+        <v>1.3572182447999999E-7</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>1</v>
@@ -6702,7 +6719,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>24</v>
@@ -6727,21 +6744,21 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="6">
-        <v>6.4204E-7</v>
+        <v>-6.4204E-7</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" ref="D20" si="10">C20*0.9</f>
-        <v>5.7783600000000004E-7</v>
+        <v>-5.7783600000000004E-7</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" ref="E20" si="11">C20*1.1</f>
-        <v>7.0624400000000006E-7</v>
+        <v>-7.0624400000000006E-7</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>1</v>
@@ -6752,22 +6769,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="2">
         <f>0.147*C37+0.1222*C35+87.3/3600*C38+2.3704*C37+0.312*C36+(1000-1000*7.8/100/101.07*207.43)/1000*C31+0.9454*C24+1000*7.8/100/1000*C32/35335*2665+1000*7.8/100/101.07*(207.43-101.07)/1000*C33+0.487*1000*7.8/100/101.07*207.43/1000*C38+2.59/1000*C34</f>
-        <v>2.2343652004299671E-5</v>
+        <v>2.2341083526699671E-5</v>
       </c>
       <c r="D21" s="2">
         <f>C21*0.9</f>
-        <v>2.0109286803869706E-5</v>
+        <v>2.0106975174029706E-5</v>
       </c>
       <c r="E21" s="2">
         <f>C21*1.1</f>
-        <v>2.4578017204729639E-5</v>
+        <v>2.457519187936964E-5</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>1</v>
@@ -6778,22 +6795,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="2">
         <f>0.4168*C36+3.358*C35+0.206*C37+1.6569*C37+0.4856*C36+0.0149*C38+1.2669*C36+0.7722*C23+0.6177*C24+0.0349*C25+0.136*C26+0.0834*C27+0.0973*C28+0.0088*C29+1.301*C30</f>
-        <v>1.3924763763789999E-6</v>
+        <v>1.374618047989E-6</v>
       </c>
       <c r="D22" s="2">
         <f>C22*0.9</f>
-        <v>1.2532287387411E-6</v>
+        <v>1.2371562431901E-6</v>
       </c>
       <c r="E22" s="2">
         <f>C22*1.1</f>
-        <v>1.5317240140169E-6</v>
+        <v>1.5120798527879002E-6</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>1</v>
@@ -6804,7 +6821,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>24</v>
@@ -6829,7 +6846,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>24</v>
@@ -6854,7 +6871,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>24</v>
@@ -6879,7 +6896,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>24</v>
@@ -6904,7 +6921,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>24</v>
@@ -6929,7 +6946,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>24</v>
@@ -6954,7 +6971,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>24</v>
@@ -6979,7 +6996,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>24</v>
@@ -7004,7 +7021,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>24</v>
@@ -7029,7 +7046,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>24</v>
@@ -7054,7 +7071,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>24</v>
@@ -7079,7 +7096,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>24</v>
@@ -7104,7 +7121,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>24</v>
@@ -7129,21 +7146,21 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C36" s="6">
-        <v>1.3243E-8</v>
+        <v>5.0106999999999997E-9</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" si="12"/>
-        <v>1.1918699999999999E-8</v>
+        <v>4.5096299999999999E-9</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="13"/>
-        <v>1.45673E-8</v>
+        <v>5.5117700000000003E-9</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>1</v>
@@ -7154,7 +7171,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>24</v>
@@ -7179,7 +7196,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>24</v>
@@ -7212,8 +7229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D808FE82-F88E-9643-85A3-7681782C4413}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7250,7 +7267,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>25</v>
@@ -7302,7 +7319,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>25</v>
@@ -7327,7 +7344,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>25</v>
@@ -7352,7 +7369,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>25</v>
@@ -7377,7 +7394,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>25</v>
@@ -7402,7 +7419,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>25</v>
@@ -7603,7 +7620,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>25</v>
@@ -7629,7 +7646,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>25</v>
@@ -7654,21 +7671,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="2">
-        <v>9.2588000000000002E-4</v>
+      <c r="C18" s="9">
+        <f>C36*24.624</f>
+        <v>9.7373145599999994E-4</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>8.3329200000000002E-4</v>
+        <v>8.7635831040000002E-4</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>1.018468E-3</v>
+        <v>1.0711046016000001E-3</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>1</v>
@@ -7679,7 +7697,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>25</v>
@@ -7704,21 +7722,21 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="2">
-        <v>1.9456E-3</v>
+        <v>-1.9456E-3</v>
       </c>
       <c r="D20" s="2">
         <f>C20*0.9</f>
-        <v>1.7510400000000001E-3</v>
+        <v>-1.7510400000000001E-3</v>
       </c>
       <c r="E20" s="2">
         <f>C20*1.1</f>
-        <v>2.1401600000000003E-3</v>
+        <v>-2.1401600000000003E-3</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>1</v>
@@ -7729,22 +7747,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="2">
         <f>0.147*C37+0.1222*C35+87.3/3600*C38+2.3704*C37+0.312*C36+(1000-1000*7.8/100/101.07*207.43)/1000*C31+0.9454*C24+1000*7.8/100/1000*C32/35335*2665+1000*7.8/100/101.07*(207.43-101.07)/1000*C33+0.487*1000*7.8/100/101.07*207.43/1000*C38+2.59/1000*C34</f>
-        <v>6.7354050717807477</v>
+        <v>6.7353796512687483</v>
       </c>
       <c r="D21" s="2">
         <f>C21*0.9</f>
-        <v>6.061864564602673</v>
+        <v>6.0618416861418734</v>
       </c>
       <c r="E21" s="2">
         <f>C21*1.1</f>
-        <v>7.4089455789588232</v>
+        <v>7.4089176163956241</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>1</v>
@@ -7755,22 +7773,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="2">
         <f>0.4168*C36+3.358*C35+0.206*C37+1.6569*C37+0.4856*C36+0.0149*C38+1.2669*C36+0.7722*C23+0.6177*C24+0.0349*C25+0.136*C26+0.0834*C27+0.0973*C28+0.0088*C29+1.301*C30</f>
-        <v>2.9648759230633998E-2</v>
+        <v>2.9472013343833998E-2</v>
       </c>
       <c r="D22" s="2">
         <f>C22*0.9</f>
-        <v>2.6683883307570599E-2</v>
+        <v>2.6524812009450598E-2</v>
       </c>
       <c r="E22" s="2">
         <f>C22*1.1</f>
-        <v>3.2613635153697404E-2</v>
+        <v>3.2419214678217401E-2</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>1</v>
@@ -7781,7 +7799,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>25</v>
@@ -7806,7 +7824,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>25</v>
@@ -7831,7 +7849,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>25</v>
@@ -7856,7 +7874,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>25</v>
@@ -7881,7 +7899,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>25</v>
@@ -7906,7 +7924,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>25</v>
@@ -7931,7 +7949,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>25</v>
@@ -7956,7 +7974,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>25</v>
@@ -7981,7 +7999,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>25</v>
@@ -8006,7 +8024,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>25</v>
@@ -8031,7 +8049,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>25</v>
@@ -8056,7 +8074,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>25</v>
@@ -8081,7 +8099,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>25</v>
@@ -8106,21 +8124,21 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="2">
-        <v>1.2102E-4</v>
+      <c r="C36" s="6">
+        <v>3.9544E-5</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" si="10"/>
-        <v>1.08918E-4</v>
+        <v>3.5589600000000002E-5</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="11"/>
-        <v>1.33122E-4</v>
+        <v>4.3498400000000004E-5</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>1</v>
@@ -8131,7 +8149,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>25</v>
@@ -8156,7 +8174,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>25</v>
@@ -8190,7 +8208,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8226,7 +8244,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>26</v>
@@ -8278,7 +8296,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>26</v>
@@ -8303,7 +8321,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>26</v>
@@ -8328,7 +8346,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>26</v>
@@ -8353,7 +8371,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>26</v>
@@ -8378,7 +8396,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>26</v>
@@ -8579,7 +8597,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>26</v>
@@ -8605,7 +8623,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>26</v>
@@ -8630,21 +8648,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="2">
-        <v>8.8329000000000001E-4</v>
+      <c r="C18" s="9">
+        <f>C36*24.624</f>
+        <v>6.6642393600000003E-4</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>7.9496100000000006E-4</v>
+        <v>5.9978154239999999E-4</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>9.7161900000000006E-4</v>
+        <v>7.3306632960000006E-4</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>1</v>
@@ -8655,7 +8674,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>26</v>
@@ -8680,21 +8699,21 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="2">
-        <v>6.9251999999999996E-4</v>
+        <v>-6.9251999999999996E-4</v>
       </c>
       <c r="D20" s="2">
         <f>C20*0.9</f>
-        <v>6.2326799999999996E-4</v>
+        <v>-6.2326799999999996E-4</v>
       </c>
       <c r="E20" s="2">
         <f>C20*1.1</f>
-        <v>7.6177199999999997E-4</v>
+        <v>-7.6177199999999997E-4</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>1</v>
@@ -8705,22 +8724,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="2">
         <f>0.147*C37+0.1222*C35+87.3/3600*C38+2.3704*C37+0.312*C36+(1000-1000*7.8/100/101.07*207.43)/1000*C31+0.9454*C24+1000*7.8/100/1000*C32/35335*2665+1000*7.8/100/101.07*(207.43-101.07)/1000*C33+0.487*1000*7.8/100/101.07*207.43/1000*C38+2.59/1000*C34</f>
-        <v>1.6167931320938957</v>
+        <v>1.6167729144938956</v>
       </c>
       <c r="D21" s="2">
         <f>C21*0.9</f>
-        <v>1.4551138188845063</v>
+        <v>1.455095623044506</v>
       </c>
       <c r="E21" s="2">
         <f>C21*1.1</f>
-        <v>1.7784724453032854</v>
+        <v>1.7784502059432854</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>1</v>
@@ -8731,22 +8750,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="2">
         <f>0.4168*C36+3.358*C35+0.206*C37+1.6569*C37+0.4856*C36+0.0149*C38+1.2669*C36+0.7722*C23+0.6177*C24+0.0349*C25+0.136*C26+0.0834*C27+0.0973*C28+0.0088*C29+1.301*C30</f>
-        <v>0.28751694505445002</v>
+        <v>0.28737637441445002</v>
       </c>
       <c r="D22" s="2">
         <f>C22*0.9</f>
-        <v>0.25876525054900501</v>
+        <v>0.25863873697300505</v>
       </c>
       <c r="E22" s="2">
         <f>C22*1.1</f>
-        <v>0.31626863955989504</v>
+        <v>0.31611401185589505</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>1</v>
@@ -8757,7 +8776,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>26</v>
@@ -8782,7 +8801,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>26</v>
@@ -8807,7 +8826,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>26</v>
@@ -8832,7 +8851,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>26</v>
@@ -8857,7 +8876,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>26</v>
@@ -8882,7 +8901,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>26</v>
@@ -8907,7 +8926,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>26</v>
@@ -8932,7 +8951,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>26</v>
@@ -8957,7 +8976,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>26</v>
@@ -8982,7 +9001,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>26</v>
@@ -9007,7 +9026,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>26</v>
@@ -9032,7 +9051,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>26</v>
@@ -9057,7 +9076,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>26</v>
@@ -9082,21 +9101,21 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="6">
-        <v>9.1864E-5</v>
+        <v>2.7064E-5</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" si="10"/>
-        <v>8.2677599999999996E-5</v>
+        <v>2.4357600000000002E-5</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="11"/>
-        <v>1.010504E-4</v>
+        <v>2.9770400000000002E-5</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>1</v>
@@ -9107,7 +9126,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>26</v>
@@ -9132,7 +9151,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>26</v>
@@ -9166,7 +9185,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9202,7 +9221,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>27</v>
@@ -9254,7 +9273,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>27</v>
@@ -9279,7 +9298,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>27</v>
@@ -9304,7 +9323,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>27</v>
@@ -9329,7 +9348,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>27</v>
@@ -9354,7 +9373,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>27</v>
@@ -9555,7 +9574,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>27</v>
@@ -9581,7 +9600,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>27</v>
@@ -9606,21 +9625,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="2">
-        <v>4.3413000000000004</v>
+      <c r="C18" s="9">
+        <f>C36*24.624</f>
+        <v>3.6320399999999995</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>3.9071700000000003</v>
+        <v>3.2688359999999994</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>4.775430000000001</v>
+        <v>3.9952439999999996</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>1</v>
@@ -9631,7 +9651,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>27</v>
@@ -9656,21 +9676,21 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="2">
-        <v>2.9281000000000001</v>
+        <v>-2.9281000000000001</v>
       </c>
       <c r="D20" s="2">
         <f>C20*0.9</f>
-        <v>2.6352900000000004</v>
+        <v>-2.6352900000000004</v>
       </c>
       <c r="E20" s="2">
         <f>C20*1.1</f>
-        <v>3.2209100000000004</v>
+        <v>-3.2209100000000004</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>1</v>
@@ -9681,22 +9701,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="2">
         <f>0.147*C37+0.1222*C35+87.3/3600*C38+2.3704*C37+0.312*C36+(1000-1000*7.8/100/101.07*207.43)/1000*C31+0.9454*C24+1000*7.8/100/1000*C32/35335*2665+1000*7.8/100/101.07*(207.43-101.07)/1000*C33+0.487*1000*7.8/100/101.07*207.43/1000*C38+2.59/1000*C34</f>
-        <v>27306.372319349357</v>
+        <v>27306.325609829357</v>
       </c>
       <c r="D21" s="2">
         <f>C21*0.9</f>
-        <v>24575.735087414421</v>
+        <v>24575.69304884642</v>
       </c>
       <c r="E21" s="2">
         <f>C21*1.1</f>
-        <v>30037.009551284296</v>
+        <v>30036.958170812293</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>1</v>
@@ -9707,22 +9727,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C22" s="2">
         <f>0.4168*C36+3.358*C35+0.206*C37+1.6569*C37+0.4856*C36+0.0149*C38+1.2669*C36+0.7722*C23+0.6177*C24+0.0349*C25+0.136*C26+0.0834*C27+0.0973*C28+0.0088*C29+1.301*C30</f>
-        <v>369.79168803089993</v>
+        <v>369.46692212789992</v>
       </c>
       <c r="D22" s="2">
         <f>C22*0.9</f>
-        <v>332.81251922780996</v>
+        <v>332.52022991510995</v>
       </c>
       <c r="E22" s="2">
         <f>C22*1.1</f>
-        <v>406.77085683398997</v>
+        <v>406.41361434068995</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>1</v>
@@ -9733,7 +9753,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>27</v>
@@ -9758,7 +9778,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>27</v>
@@ -9783,7 +9803,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>27</v>
@@ -9808,7 +9828,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>27</v>
@@ -9833,7 +9853,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>27</v>
@@ -9858,7 +9878,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>27</v>
@@ -9883,7 +9903,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>27</v>
@@ -9908,7 +9928,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>27</v>
@@ -9933,7 +9953,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>27</v>
@@ -9958,7 +9978,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>27</v>
@@ -9983,7 +10003,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>27</v>
@@ -10008,7 +10028,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>27</v>
@@ -10033,7 +10053,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>27</v>
@@ -10058,21 +10078,21 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C36" s="2">
-        <v>0.29720999999999997</v>
+        <v>0.14749999999999999</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" si="10"/>
-        <v>0.26748899999999998</v>
+        <v>0.13275000000000001</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="11"/>
-        <v>0.32693099999999997</v>
+        <v>0.16225000000000001</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>1</v>
@@ -10083,7 +10103,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>27</v>
@@ -10108,7 +10128,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
add LCA metrics; change MFSP to MDSP
</commit_message>
<xml_diff>
--- a/exposan/htl/data/impact_items.xlsx
+++ b/exposan/htl/data/impact_items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiananfeng/Desktop/PhD CEE/coding/Cloned packages/EXPOsan/exposan/htl/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiananfeng/Desktop/PhD_CEE/coding/cloned_packages/EXPOsan/exposan/htl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B50152-10B7-254B-B784-312D689FF9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544AB7EC-3193-B546-914B-2126EABE5748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11240" yWindow="4660" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="20220" yWindow="3160" windowWidth="28800" windowHeight="17500" activeTab="9" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="RespiratoryEffects" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029" iterate="1" iterateCount="25"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="109">
   <si>
     <t>ecoinvent 3</t>
   </si>
@@ -364,6 +365,12 @@
   </si>
   <si>
     <t>includle burning emission, 1 kg natural gas = 24.624 MJ (see Ecoinvent: market for natural gas liquids)</t>
+  </si>
+  <si>
+    <t>market for naphtha</t>
+  </si>
+  <si>
+    <t>Napatha</t>
   </si>
 </sst>
 </file>
@@ -424,15 +431,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -750,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66379A7A-E84B-1346-816F-577916F7D6A6}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C11" sqref="A11:XFD11"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -817,11 +821,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -830,13 +834,12 @@
       <c r="D4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>80</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -845,7 +848,6 @@
       <c r="D5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -923,17 +925,17 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1082,11 +1084,11 @@
       <c r="B21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -1095,11 +1097,11 @@
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
@@ -1335,6 +1337,20 @@
       </c>
       <c r="E38" s="2" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1348,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32918E97-33AC-4743-867D-87B08CF8DB3F}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1406,10 +1422,10 @@
         <f t="shared" ref="E2:E15" si="1">C2*1.1</f>
         <v>2.9457343110642956E-3</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1432,15 +1448,15 @@
         <f t="shared" si="1"/>
         <v>8.5052000000000012E-5</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1457,15 +1473,15 @@
         <f t="shared" si="1"/>
         <v>3.1801000000000004</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1482,7 +1498,7 @@
         <f t="shared" ref="E5" si="3">C5*1.1</f>
         <v>52.043199999999999</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -1507,10 +1523,10 @@
         <f t="shared" si="1"/>
         <v>1.8536100000000003E-2</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1532,7 +1548,7 @@
         <f t="shared" si="1"/>
         <v>3.5095500000000006E-3</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -1557,7 +1573,7 @@
         <f t="shared" ref="E8" si="4">C8*1.1</f>
         <v>3.5418900000000002E-3</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1582,7 +1598,7 @@
         <f t="shared" si="1"/>
         <v>3.1655799999999999E-3</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -1596,7 +1612,7 @@
       <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <f>0.001868/20+19/20*C24</f>
         <v>9.405486350000001E-5</v>
       </c>
@@ -1608,7 +1624,7 @@
         <f t="shared" si="1"/>
         <v>1.0346034985000002E-4</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -1633,7 +1649,7 @@
         <f t="shared" si="1"/>
         <v>4.8235000000000005E-3</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -1658,7 +1674,7 @@
         <f t="shared" si="1"/>
         <v>4.0367800000000002E-3</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -1683,7 +1699,7 @@
         <f t="shared" si="1"/>
         <v>9.6305000000000002E-4</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -1708,7 +1724,7 @@
         <f t="shared" si="1"/>
         <v>2.69973E-3</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -1733,10 +1749,10 @@
         <f t="shared" si="1"/>
         <v>2.02257E-3</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1759,7 +1775,7 @@
         <f t="shared" ref="E16:E17" si="7">C16*1.1</f>
         <v>-6.7940399372478722E-4</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -1784,7 +1800,7 @@
         <f t="shared" si="7"/>
         <v>-3.4446500000000005E-3</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -1798,7 +1814,7 @@
       <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="2">
         <f>C36*24.624</f>
         <v>3.50916624E-4</v>
       </c>
@@ -1810,7 +1826,7 @@
         <f>C18*1.1</f>
         <v>3.8600828640000004E-4</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -1835,7 +1851,7 @@
         <f>C19*1.1</f>
         <v>1.4737800000000001E-3</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -1860,7 +1876,7 @@
         <f>C20*1.1</f>
         <v>-1.2205600000000001E-3</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -1886,7 +1902,7 @@
         <f>C21*1.1</f>
         <v>3.8688976176372694</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -1912,7 +1928,7 @@
         <f>C22*1.1</f>
         <v>2.2852949798405103E-2</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -1937,7 +1953,7 @@
         <f t="shared" ref="E23:E38" si="9">C23*1.1</f>
         <v>3.0585500000000002E-3</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -1951,7 +1967,7 @@
       <c r="B24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="4">
         <v>6.8932999999999999E-7</v>
       </c>
       <c r="D24" s="2">
@@ -1962,7 +1978,7 @@
         <f t="shared" si="9"/>
         <v>7.5826300000000004E-7</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -1987,7 +2003,7 @@
         <f t="shared" si="9"/>
         <v>4.941860000000001E-3</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -2012,7 +2028,7 @@
         <f t="shared" si="9"/>
         <v>6.5347700000000009E-2</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -2037,7 +2053,7 @@
         <f t="shared" si="9"/>
         <v>0.10944780000000001</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -2062,7 +2078,7 @@
         <f t="shared" si="9"/>
         <v>2.4799500000000003E-3</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -2087,7 +2103,7 @@
         <f t="shared" si="9"/>
         <v>4.0367800000000002E-3</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -2112,7 +2128,7 @@
         <f t="shared" si="9"/>
         <v>1.2205600000000001E-3</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -2137,7 +2153,7 @@
         <f t="shared" si="9"/>
         <v>5.3810900000000007E-3</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
@@ -2162,7 +2178,7 @@
         <f t="shared" si="9"/>
         <v>656.78800000000012</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -2187,7 +2203,7 @@
         <f t="shared" si="9"/>
         <v>2.10254E-3</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -2212,7 +2228,7 @@
         <f t="shared" si="9"/>
         <v>9.3168900000000008E-4</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -2226,7 +2242,7 @@
       <c r="B35" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="4">
         <v>5.0587999999999997E-5</v>
       </c>
       <c r="D35" s="2">
@@ -2237,7 +2253,7 @@
         <f t="shared" si="9"/>
         <v>5.5646800000000004E-5</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -2251,7 +2267,7 @@
       <c r="B36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="4">
         <v>1.4251E-5</v>
       </c>
       <c r="D36" s="2">
@@ -2262,7 +2278,7 @@
         <f t="shared" si="9"/>
         <v>1.5676100000000001E-5</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -2276,7 +2292,7 @@
       <c r="B37" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="4">
         <v>9.5338000000000001E-5</v>
       </c>
       <c r="D37" s="2">
@@ -2287,7 +2303,7 @@
         <f t="shared" si="9"/>
         <v>1.0487180000000001E-4</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G37" s="2" t="s">
@@ -2312,10 +2328,35 @@
         <f t="shared" si="9"/>
         <v>1.4737800000000001E-3</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="2">
+        <v>9.4609999999999996E-4</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" ref="D39" si="10">C39*0.9</f>
+        <v>8.5148999999999999E-4</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" ref="E39" si="11">C39*1.1</f>
+        <v>1.04071E-3</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2328,10 +2369,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B44E52-5A7F-8142-BD9E-CE1C29D2C0B8}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="106" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A8" zoomScale="106" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2386,10 +2427,10 @@
         <f t="shared" ref="E2:E14" si="1">C2*1.1</f>
         <v>0.50242944536725687</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2412,15 +2453,15 @@
         <f t="shared" si="1"/>
         <v>2.145704E-2</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2437,15 +2478,15 @@
         <f t="shared" si="1"/>
         <v>585.83800000000008</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2462,7 +2503,7 @@
         <f t="shared" ref="E5" si="3">C5*1.1</f>
         <v>9145.84</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -2487,10 +2528,10 @@
         <f t="shared" si="1"/>
         <v>1.4276900000000001</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2512,7 +2553,7 @@
         <f t="shared" si="1"/>
         <v>0.445687</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -2537,7 +2578,7 @@
         <f t="shared" ref="E8" si="5">C8*1.1</f>
         <v>0.45448700000000003</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -2562,7 +2603,7 @@
         <f t="shared" si="1"/>
         <v>0.58886300000000003</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -2588,7 +2629,7 @@
         <f t="shared" si="1"/>
         <v>2.16468142E-2</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -2613,7 +2654,7 @@
         <f t="shared" si="1"/>
         <v>0.84717600000000004</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -2638,7 +2679,7 @@
         <f t="shared" si="1"/>
         <v>0.891154</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -2663,7 +2704,7 @@
         <f t="shared" si="1"/>
         <v>0.13842400000000002</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -2688,7 +2729,7 @@
         <f t="shared" si="1"/>
         <v>0.37021600000000005</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -2713,10 +2754,10 @@
         <f>C15*1.1</f>
         <v>0.38150200000000006</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2739,10 +2780,10 @@
         <f t="shared" ref="E16:E17" si="7">C16*1.1</f>
         <v>-0.13511255714926043</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="5" t="s">
+      <c r="F16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2764,10 +2805,10 @@
         <f t="shared" si="7"/>
         <v>-0.80208699999999999</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2790,7 +2831,7 @@
         <f>C18*1.1</f>
         <v>9.2204814240000002E-2</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -2815,7 +2856,7 @@
         <f>C19*1.1</f>
         <v>0.17380000000000001</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -2840,7 +2881,7 @@
         <f t="shared" ref="E20" si="9">C20*1.1</f>
         <v>-0.27680399999999999</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -2866,7 +2907,7 @@
         <f>C21*1.1</f>
         <v>1090.8180786844227</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -2892,7 +2933,7 @@
         <f>C22*1.1</f>
         <v>4.4496451845802012</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -2917,7 +2958,7 @@
         <f t="shared" ref="E23:E34" si="11">C23*1.1</f>
         <v>0.65946100000000007</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -2942,7 +2983,7 @@
         <f t="shared" si="11"/>
         <v>1.28436E-4</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -2967,7 +3008,7 @@
         <f t="shared" si="11"/>
         <v>0.95753900000000003</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -2992,7 +3033,7 @@
         <f t="shared" si="11"/>
         <v>11.6919</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -3017,7 +3058,7 @@
         <f t="shared" si="11"/>
         <v>21.763500000000001</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -3042,7 +3083,7 @@
         <f t="shared" si="11"/>
         <v>0.52683400000000002</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -3067,7 +3108,7 @@
         <f t="shared" si="11"/>
         <v>0.891154</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -3092,7 +3133,7 @@
         <f t="shared" si="11"/>
         <v>0.27680399999999999</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -3117,7 +3158,7 @@
         <f t="shared" si="11"/>
         <v>1.093774</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
@@ -3142,7 +3183,7 @@
         <f t="shared" si="11"/>
         <v>185251.00000000003</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -3167,7 +3208,7 @@
         <f t="shared" si="11"/>
         <v>0.26710200000000001</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -3192,7 +3233,7 @@
         <f t="shared" si="11"/>
         <v>0.10837750000000002</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -3217,7 +3258,7 @@
         <f t="shared" ref="E35:E37" si="12">C35*1.1</f>
         <v>9.0780800000000005E-3</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -3242,7 +3283,7 @@
         <f t="shared" si="12"/>
         <v>3.7445100000000004E-3</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -3267,7 +3308,7 @@
         <f t="shared" si="12"/>
         <v>2.2178200000000002E-2</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G37" s="2" t="s">
@@ -3292,10 +3333,35 @@
         <f>C38*1.1</f>
         <v>0.17380000000000001</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="2">
+        <v>-0.21812999999999999</v>
+      </c>
+      <c r="D39" s="2">
+        <f>C39*0.9</f>
+        <v>-0.19631699999999999</v>
+      </c>
+      <c r="E39" s="2">
+        <f>C39*1.1</f>
+        <v>-0.23994300000000002</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3307,10 +3373,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB3A8C1-31D1-8447-9043-3E804D12662D}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="B38" sqref="B38:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3363,10 +3429,10 @@
         <f t="shared" ref="E2:E3" si="1">C2*1.1</f>
         <v>2.7546303123607343</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3389,15 +3455,15 @@
         <f t="shared" si="1"/>
         <v>5.3719600000000006E-2</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3414,15 +3480,15 @@
         <f t="shared" ref="E4:E17" si="3">C4*1.1</f>
         <v>4110.4800000000005</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -3439,7 +3505,7 @@
         <f t="shared" ref="E5" si="5">C5*1.1</f>
         <v>63232.400000000009</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -3464,10 +3530,10 @@
         <f t="shared" si="3"/>
         <v>7.9239600000000001</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3489,7 +3555,7 @@
         <f t="shared" si="3"/>
         <v>2.2299200000000003</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -3514,7 +3580,7 @@
         <f t="shared" si="3"/>
         <v>1.8992599999999999</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -3539,7 +3605,7 @@
         <f t="shared" si="3"/>
         <v>0.99932799999999999</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -3565,7 +3631,7 @@
         <f t="shared" si="3"/>
         <v>7.6900279500000002E-2</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -3590,7 +3656,7 @@
         <f t="shared" si="3"/>
         <v>1.0766580000000001</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -3615,7 +3681,7 @@
         <f t="shared" si="3"/>
         <v>0.47021700000000005</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -3640,7 +3706,7 @@
         <f t="shared" si="3"/>
         <v>3.0743900000000006</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -3665,7 +3731,7 @@
         <f t="shared" si="3"/>
         <v>0.84999200000000008</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -3690,10 +3756,10 @@
         <f t="shared" si="3"/>
         <v>0.9933550000000001</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3716,10 +3782,10 @@
         <f t="shared" si="3"/>
         <v>-0.29656703585835947</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="5" t="s">
+      <c r="F16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3741,10 +3807,10 @@
         <f t="shared" si="3"/>
         <v>-3.8220600000000005</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3767,7 +3833,7 @@
         <f>C18*1.1</f>
         <v>6.979081824000001E-2</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -3792,7 +3858,7 @@
         <f>C19*1.1</f>
         <v>0.29330400000000001</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -3817,7 +3883,7 @@
         <f t="shared" ref="E20" si="7">C20*1.1</f>
         <v>-0.20622800000000002</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -3843,7 +3909,7 @@
         <f>C21*1.1</f>
         <v>16908.189694727098</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -3869,7 +3935,7 @@
         <f>C22*1.1</f>
         <v>55.285610373785012</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -3894,7 +3960,7 @@
         <f t="shared" ref="E23:E37" si="9">C23*1.1</f>
         <v>1.8956300000000001</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -3919,7 +3985,7 @@
         <f t="shared" si="9"/>
         <v>5.5166099999999999E-3</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -3944,7 +4010,7 @@
         <f t="shared" si="9"/>
         <v>2.7680400000000001</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -3969,7 +4035,7 @@
         <f t="shared" si="9"/>
         <v>333.49800000000005</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -3994,7 +4060,7 @@
         <f t="shared" si="9"/>
         <v>94.496600000000015</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -4019,7 +4085,7 @@
         <f t="shared" si="9"/>
         <v>3.0835200000000004E-2</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -4044,7 +4110,7 @@
         <f t="shared" si="9"/>
         <v>0.47021700000000005</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -4069,7 +4135,7 @@
         <f t="shared" si="9"/>
         <v>0.20622800000000002</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -4094,7 +4160,7 @@
         <f t="shared" si="9"/>
         <v>3.3399300000000007</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
@@ -4119,7 +4185,7 @@
         <f t="shared" si="9"/>
         <v>2873640</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -4144,7 +4210,7 @@
         <f t="shared" si="9"/>
         <v>0.63273100000000004</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -4169,7 +4235,7 @@
         <f t="shared" si="9"/>
         <v>0.18491000000000002</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -4194,7 +4260,7 @@
         <f t="shared" si="9"/>
         <v>2.83371E-2</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -4219,7 +4285,7 @@
         <f t="shared" si="9"/>
         <v>2.8342600000000003E-3</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -4244,7 +4310,7 @@
         <f t="shared" si="9"/>
         <v>5.5790900000000004E-2</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G37" s="2" t="s">
@@ -4269,10 +4335,35 @@
         <f>C38*1.1</f>
         <v>0.29330400000000001</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.15887000000000001</v>
+      </c>
+      <c r="D39" s="2">
+        <f>C39*0.9</f>
+        <v>0.14298300000000003</v>
+      </c>
+      <c r="E39" s="2">
+        <f>C39*1.1</f>
+        <v>0.17475700000000002</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4284,10 +4375,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CC6322-9D61-AD41-A8B1-E5A60BE6F0EB}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4341,10 +4432,10 @@
         <f t="shared" ref="E2:E5" si="1">C2*1.1</f>
         <v>5.1957452497670465E-4</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4367,15 +4458,15 @@
         <f t="shared" si="1"/>
         <v>2.6544760000000004E-5</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -4392,15 +4483,15 @@
         <f t="shared" si="1"/>
         <v>0.29117000000000004</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -4417,7 +4508,7 @@
         <f t="shared" si="1"/>
         <v>4.6984300000000001</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -4442,10 +4533,10 @@
         <f t="shared" ref="E6:E15" si="3">C6*1.1</f>
         <v>9.1539799999999999E-4</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4467,7 +4558,7 @@
         <f t="shared" si="3"/>
         <v>6.6471900000000003E-4</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -4492,7 +4583,7 @@
         <f t="shared" ref="E8" si="5">C8*1.1</f>
         <v>5.3142100000000002E-4</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -4517,7 +4608,7 @@
         <f t="shared" si="3"/>
         <v>3.1154200000000003E-3</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -4531,7 +4622,7 @@
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <f>0.000079544/20+19/20*C24</f>
         <v>4.0466411999999999E-6</v>
       </c>
@@ -4543,7 +4634,7 @@
         <f t="shared" si="3"/>
         <v>4.4513053199999999E-6</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -4568,7 +4659,7 @@
         <f t="shared" si="3"/>
         <v>4.3743699999999999E-4</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -4593,7 +4684,7 @@
         <f t="shared" si="3"/>
         <v>3.2356500000000005E-3</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -4618,7 +4709,7 @@
         <f t="shared" si="3"/>
         <v>6.99677E-4</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -4643,7 +4734,7 @@
         <f t="shared" si="3"/>
         <v>3.6198799999999999E-4</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -4668,10 +4759,10 @@
         <f t="shared" si="3"/>
         <v>5.211910000000001E-3</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4694,10 +4785,10 @@
         <f t="shared" ref="E16" si="7">C16*1.1</f>
         <v>-1.924470977140296E-4</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="5" t="s">
+      <c r="F16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4719,10 +4810,10 @@
         <f t="shared" ref="E17" si="9">C17*1.1</f>
         <v>-2.7096300000000002E-3</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4733,7 +4824,7 @@
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="4">
         <f>C36*24.624</f>
         <v>7.2539841599999995E-5</v>
       </c>
@@ -4745,7 +4836,7 @@
         <f>C18*1.1</f>
         <v>7.9793825759999997E-5</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -4759,7 +4850,7 @@
       <c r="B19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="4">
         <v>9.4215000000000005E-5</v>
       </c>
       <c r="D19" s="2">
@@ -4770,7 +4861,7 @@
         <f>C19*1.1</f>
         <v>1.0363650000000002E-4</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -4795,7 +4886,7 @@
         <f>C20*1.1</f>
         <v>-1.1601700000000001E-3</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -4821,7 +4912,7 @@
         <f>C21*1.1</f>
         <v>0.49521127543041399</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -4847,7 +4938,7 @@
         <f>C22*1.1</f>
         <v>6.3244046626961198E-3</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -4865,14 +4956,14 @@
         <v>4.2278999999999998E-4</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" ref="D23:D38" si="10">C23*0.9</f>
+        <f t="shared" ref="D23:D39" si="10">C23*0.9</f>
         <v>3.8051099999999999E-4</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" ref="E23:E38" si="11">C23*1.1</f>
+        <f t="shared" ref="E23:E39" si="11">C23*1.1</f>
         <v>4.6506900000000003E-4</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -4886,7 +4977,7 @@
       <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="4">
         <v>7.3095999999999995E-8</v>
       </c>
       <c r="D24" s="2">
@@ -4897,7 +4988,7 @@
         <f t="shared" si="11"/>
         <v>8.0405600000000004E-8</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -4922,7 +5013,7 @@
         <f t="shared" si="11"/>
         <v>7.29355E-4</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -4947,7 +5038,7 @@
         <f t="shared" si="11"/>
         <v>8.6628300000000016E-3</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -4972,7 +5063,7 @@
         <f t="shared" si="11"/>
         <v>3.7845500000000004E-2</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -4986,7 +5077,7 @@
       <c r="B28" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="4">
         <v>4.1992E-5</v>
       </c>
       <c r="D28" s="2">
@@ -4997,7 +5088,7 @@
         <f t="shared" si="11"/>
         <v>4.6191200000000006E-5</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -5022,7 +5113,7 @@
         <f t="shared" si="11"/>
         <v>3.2356500000000005E-3</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -5047,7 +5138,7 @@
         <f t="shared" si="11"/>
         <v>1.1601700000000001E-3</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -5072,7 +5163,7 @@
         <f t="shared" si="11"/>
         <v>4.6601500000000007E-4</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
@@ -5097,7 +5188,7 @@
         <f t="shared" si="11"/>
         <v>84.099400000000003</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -5122,7 +5213,7 @@
         <f t="shared" si="11"/>
         <v>2.5135000000000001E-4</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -5136,7 +5227,7 @@
       <c r="B34" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="4">
         <v>6.1297999999999995E-5</v>
       </c>
       <c r="D34" s="2">
@@ -5147,7 +5238,7 @@
         <f t="shared" si="11"/>
         <v>6.7427800000000005E-5</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -5161,7 +5252,7 @@
       <c r="B35" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="4">
         <v>5.9869999999999996E-6</v>
       </c>
       <c r="D35" s="2">
@@ -5172,7 +5263,7 @@
         <f t="shared" si="11"/>
         <v>6.5857000000000003E-6</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -5186,7 +5277,7 @@
       <c r="B36" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="4">
         <v>2.9459E-6</v>
       </c>
       <c r="D36" s="2">
@@ -5197,7 +5288,7 @@
         <f t="shared" si="11"/>
         <v>3.2404900000000003E-6</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -5211,7 +5302,7 @@
       <c r="B37" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="4">
         <v>1.5750999999999999E-5</v>
       </c>
       <c r="D37" s="2">
@@ -5222,7 +5313,7 @@
         <f t="shared" si="11"/>
         <v>1.73261E-5</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G37" s="2" t="s">
@@ -5236,7 +5327,7 @@
       <c r="B38" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="4">
         <v>9.4215000000000005E-5</v>
       </c>
       <c r="D38" s="2">
@@ -5247,10 +5338,35 @@
         <f t="shared" si="11"/>
         <v>1.0363650000000002E-4</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1.0594000000000001E-3</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" ref="D39" si="12">C39*0.9</f>
+        <v>9.5346000000000005E-4</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" ref="E39" si="13">C39*1.1</f>
+        <v>1.1653400000000002E-3</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5262,10 +5378,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE2E960-887B-1E49-80AF-9619BDC224B9}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5317,10 +5433,10 @@
         <f t="shared" ref="E2:E5" si="1">C2*1.1</f>
         <v>1.3860000000000001</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5343,15 +5459,15 @@
         <f t="shared" si="1"/>
         <v>0.12424280000000001</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -5368,15 +5484,15 @@
         <f t="shared" si="1"/>
         <v>737.19799999999998</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -5393,7 +5509,7 @@
         <f t="shared" si="1"/>
         <v>13794.000000000002</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -5418,10 +5534,10 @@
         <f t="shared" ref="E6:E15" si="3">C6*1.1</f>
         <v>5.3418200000000011</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5443,7 +5559,7 @@
         <f t="shared" si="3"/>
         <v>2.2030800000000004</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -5468,7 +5584,7 @@
         <f t="shared" ref="E8" si="5">C8*1.1</f>
         <v>2.3859000000000004</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -5493,7 +5609,7 @@
         <f t="shared" si="3"/>
         <v>2.4929300000000003</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -5519,7 +5635,7 @@
         <f t="shared" si="3"/>
         <v>9.0262326000000014E-3</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -5544,7 +5660,7 @@
         <f t="shared" si="3"/>
         <v>3.1656900000000001</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -5569,7 +5685,7 @@
         <f t="shared" si="3"/>
         <v>1.7186400000000002</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -5594,7 +5710,7 @@
         <f t="shared" si="3"/>
         <v>1.2766600000000001</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -5619,7 +5735,7 @@
         <f t="shared" si="3"/>
         <v>1.3765400000000001</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -5644,10 +5760,10 @@
         <f t="shared" si="3"/>
         <v>1.6775</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5670,10 +5786,10 @@
         <f t="shared" ref="E16:E17" si="7">C16*1.1</f>
         <v>-0.46293516718960115</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="5" t="s">
+      <c r="F16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5695,10 +5811,10 @@
         <f t="shared" si="7"/>
         <v>-1.3748900000000002</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5709,7 +5825,7 @@
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="2">
         <f>C36*24.624</f>
         <v>1.584234288</v>
       </c>
@@ -5721,7 +5837,7 @@
         <f>C18*1.1</f>
         <v>1.7426577168000001</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -5746,7 +5862,7 @@
         <f>C19*1.1</f>
         <v>0.74632799999999999</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -5771,7 +5887,7 @@
         <f>C20*1.1</f>
         <v>-0.52463400000000004</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -5797,7 +5913,7 @@
         <f>C21*1.1</f>
         <v>533.23548677588883</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -5823,7 +5939,7 @@
         <f>C22*1.1</f>
         <v>6.8091260209016014</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -5848,7 +5964,7 @@
         <f t="shared" ref="E23:E37" si="9">C23*1.1</f>
         <v>1.75736</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -5873,7 +5989,7 @@
         <f t="shared" si="9"/>
         <v>3.3250800000000002E-4</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -5898,7 +6014,7 @@
         <f t="shared" si="9"/>
         <v>1.46201</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -5923,7 +6039,7 @@
         <f t="shared" si="9"/>
         <v>8.7334500000000013</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -5948,7 +6064,7 @@
         <f t="shared" si="9"/>
         <v>34.158300000000004</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -5973,7 +6089,7 @@
         <f t="shared" si="9"/>
         <v>0.13655400000000001</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -5998,7 +6114,7 @@
         <f t="shared" si="9"/>
         <v>1.7186400000000002</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -6023,7 +6139,7 @@
         <f t="shared" si="9"/>
         <v>0.52463400000000004</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -6048,7 +6164,7 @@
         <f t="shared" si="9"/>
         <v>3.2997800000000002</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
@@ -6073,7 +6189,7 @@
         <f t="shared" si="9"/>
         <v>90082.3</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -6098,7 +6214,7 @@
         <f t="shared" si="9"/>
         <v>1.0358040000000002</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -6123,7 +6239,7 @@
         <f t="shared" si="9"/>
         <v>0.461758</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -6148,7 +6264,7 @@
         <f t="shared" si="9"/>
         <v>7.2636300000000001E-2</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -6173,7 +6289,7 @@
         <f t="shared" si="9"/>
         <v>7.0770700000000006E-2</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -6198,7 +6314,7 @@
         <f t="shared" si="9"/>
         <v>0.131406</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G37" s="2" t="s">
@@ -6223,10 +6339,35 @@
         <f>C38*1.1</f>
         <v>0.74632799999999999</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.36864999999999998</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" ref="D39" si="10">C39*0.9</f>
+        <v>0.331785</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" ref="E39" si="11">C39*1.1</f>
+        <v>0.40551500000000001</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6238,10 +6379,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578089A2-98D2-704F-AF44-C2497A6C7B0D}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6295,10 +6436,10 @@
         <f t="shared" ref="E2:E3" si="1">C2*1.1</f>
         <v>7.9002131021350716E-8</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6309,7 +6450,7 @@
       <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="4">
         <f>0.000015044/2500</f>
         <v>6.0176000000000004E-9</v>
       </c>
@@ -6321,21 +6462,21 @@
         <f t="shared" si="1"/>
         <v>6.619360000000001E-9</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>4.5494999999999997E-5</v>
       </c>
       <c r="D4" s="2">
@@ -6346,15 +6487,15 @@
         <f t="shared" ref="E4:E15" si="3">C4*1.1</f>
         <v>5.0044499999999998E-5</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -6371,7 +6512,7 @@
         <f t="shared" ref="E5" si="5">C5*1.1</f>
         <v>8.5409500000000014E-4</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -6385,7 +6526,7 @@
       <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>1.9641E-7</v>
       </c>
       <c r="D6" s="2">
@@ -6396,10 +6537,10 @@
         <f t="shared" si="3"/>
         <v>2.1605100000000001E-7</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6410,7 +6551,7 @@
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <v>8.7602999999999994E-8</v>
       </c>
       <c r="D7" s="2">
@@ -6421,7 +6562,7 @@
         <f t="shared" si="3"/>
         <v>9.6363300000000004E-8</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -6435,7 +6576,7 @@
       <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>1.0173E-7</v>
       </c>
       <c r="D8" s="2">
@@ -6446,7 +6587,7 @@
         <f t="shared" ref="E8" si="7">C8*1.1</f>
         <v>1.1190300000000001E-7</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -6460,7 +6601,7 @@
       <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <v>2.5540999999999998E-7</v>
       </c>
       <c r="D9" s="2">
@@ -6471,7 +6612,7 @@
         <f t="shared" si="3"/>
         <v>2.8095100000000001E-7</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -6485,7 +6626,7 @@
       <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <f>0.000000014828/20+19/20*C24</f>
         <v>8.9441650000000002E-10</v>
       </c>
@@ -6497,7 +6638,7 @@
         <f t="shared" si="3"/>
         <v>9.8385815000000019E-10</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -6511,7 +6652,7 @@
       <c r="B11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <v>4.9409999999999997E-8</v>
       </c>
       <c r="D11" s="2">
@@ -6522,7 +6663,7 @@
         <f t="shared" si="3"/>
         <v>5.4351000000000001E-8</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -6536,7 +6677,7 @@
       <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>1.801E-6</v>
       </c>
       <c r="D12" s="2">
@@ -6547,7 +6688,7 @@
         <f t="shared" si="3"/>
         <v>1.9811E-6</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -6561,7 +6702,7 @@
       <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <v>1.5364000000000001E-8</v>
       </c>
       <c r="D13" s="2">
@@ -6572,7 +6713,7 @@
         <f t="shared" si="3"/>
         <v>1.6900400000000004E-8</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -6586,7 +6727,7 @@
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="4">
         <v>7.8932000000000003E-7</v>
       </c>
       <c r="D14" s="2">
@@ -6597,7 +6738,7 @@
         <f t="shared" si="3"/>
         <v>8.6825200000000006E-7</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -6611,7 +6752,7 @@
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="4">
         <v>9.2182999999999999E-8</v>
       </c>
       <c r="D15" s="2">
@@ -6622,10 +6763,10 @@
         <f t="shared" si="3"/>
         <v>1.0140130000000001E-7</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6648,10 +6789,10 @@
         <f t="shared" ref="E16:E17" si="9">C16*1.1</f>
         <v>-2.5250399775885256E-8</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="5" t="s">
+      <c r="F16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6662,7 +6803,7 @@
       <c r="B17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="4">
         <v>-6.1237999999999996E-8</v>
       </c>
       <c r="D17" s="2">
@@ -6673,10 +6814,10 @@
         <f t="shared" si="9"/>
         <v>-6.7361800000000007E-8</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6687,7 +6828,7 @@
       <c r="B18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="2">
         <f>C36*24.624</f>
         <v>1.2338347679999998E-7</v>
       </c>
@@ -6699,7 +6840,7 @@
         <f>C18*1.1</f>
         <v>1.3572182447999999E-7</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -6713,7 +6854,7 @@
       <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="4">
         <v>2.0158000000000001E-8</v>
       </c>
       <c r="D19" s="2">
@@ -6724,7 +6865,7 @@
         <f>C19*1.1</f>
         <v>2.2173800000000003E-8</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -6738,7 +6879,7 @@
       <c r="B20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="4">
         <v>-6.4204E-7</v>
       </c>
       <c r="D20" s="2">
@@ -6749,7 +6890,7 @@
         <f t="shared" ref="E20" si="11">C20*1.1</f>
         <v>-7.0624400000000006E-7</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -6775,7 +6916,7 @@
         <f>C21*1.1</f>
         <v>2.457519187936964E-5</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -6801,7 +6942,7 @@
         <f>C22*1.1</f>
         <v>1.5120798527879002E-6</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -6815,7 +6956,7 @@
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="4">
         <v>1.4991E-7</v>
       </c>
       <c r="D23" s="2">
@@ -6826,7 +6967,7 @@
         <f t="shared" ref="E23:E38" si="13">C23*1.1</f>
         <v>1.64901E-7</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -6840,7 +6981,7 @@
       <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="4">
         <v>1.6106999999999999E-10</v>
       </c>
       <c r="D24" s="2">
@@ -6851,7 +6992,7 @@
         <f t="shared" si="13"/>
         <v>1.77177E-10</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -6865,7 +7006,7 @@
       <c r="B25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="4">
         <v>1.4737999999999999E-7</v>
       </c>
       <c r="D25" s="2">
@@ -6876,7 +7017,7 @@
         <f t="shared" si="13"/>
         <v>1.62118E-7</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -6890,7 +7031,7 @@
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="4">
         <v>3.0492000000000001E-7</v>
       </c>
       <c r="D26" s="2">
@@ -6901,7 +7042,7 @@
         <f t="shared" si="13"/>
         <v>3.3541200000000001E-7</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -6915,7 +7056,7 @@
       <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="4">
         <v>3.7824E-6</v>
       </c>
       <c r="D27" s="2">
@@ -6926,7 +7067,7 @@
         <f t="shared" si="13"/>
         <v>4.1606400000000007E-6</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -6940,7 +7081,7 @@
       <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="4">
         <v>1.5302E-8</v>
       </c>
       <c r="D28" s="2">
@@ -6951,7 +7092,7 @@
         <f t="shared" si="13"/>
         <v>1.6832200000000002E-8</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -6965,7 +7106,7 @@
       <c r="B29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="4">
         <v>1.801E-6</v>
       </c>
       <c r="D29" s="2">
@@ -6976,7 +7117,7 @@
         <f t="shared" si="13"/>
         <v>1.9811E-6</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -6990,7 +7131,7 @@
       <c r="B30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="4">
         <v>6.4204E-7</v>
       </c>
       <c r="D30" s="2">
@@ -7001,7 +7142,7 @@
         <f t="shared" si="13"/>
         <v>7.0624400000000006E-7</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -7015,7 +7156,7 @@
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="4">
         <v>8.8093999999999995E-8</v>
       </c>
       <c r="D31" s="2">
@@ -7026,7 +7167,7 @@
         <f t="shared" si="13"/>
         <v>9.6903399999999999E-8</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
@@ -7051,7 +7192,7 @@
         <f t="shared" si="13"/>
         <v>4.14986E-3</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -7065,7 +7206,7 @@
       <c r="B33" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="4">
         <v>5.7080999999999996E-7</v>
       </c>
       <c r="D33" s="2">
@@ -7076,7 +7217,7 @@
         <f t="shared" si="13"/>
         <v>6.2789100000000002E-7</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -7090,7 +7231,7 @@
       <c r="B34" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="4">
         <v>1.092E-8</v>
       </c>
       <c r="D34" s="2">
@@ -7101,7 +7242,7 @@
         <f t="shared" si="13"/>
         <v>1.2012E-8</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -7115,7 +7256,7 @@
       <c r="B35" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="4">
         <v>4.8915999999999999E-9</v>
       </c>
       <c r="D35" s="2">
@@ -7126,7 +7267,7 @@
         <f t="shared" si="13"/>
         <v>5.3807600000000008E-9</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -7140,7 +7281,7 @@
       <c r="B36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="4">
         <v>5.0106999999999997E-9</v>
       </c>
       <c r="D36" s="2">
@@ -7151,7 +7292,7 @@
         <f t="shared" si="13"/>
         <v>5.5117700000000003E-9</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -7165,7 +7306,7 @@
       <c r="B37" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="4">
         <v>8.8386000000000005E-9</v>
       </c>
       <c r="D37" s="2">
@@ -7176,7 +7317,7 @@
         <f t="shared" si="13"/>
         <v>9.722460000000002E-9</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G37" s="2" t="s">
@@ -7190,7 +7331,7 @@
       <c r="B38" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="4">
         <v>2.0158000000000001E-8</v>
       </c>
       <c r="D38" s="2">
@@ -7201,10 +7342,35 @@
         <f t="shared" si="13"/>
         <v>2.2173800000000003E-8</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="4">
+        <v>6.4977000000000003E-7</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" ref="D39" si="14">C39*0.9</f>
+        <v>5.8479300000000001E-7</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" ref="E39" si="15">C39*1.1</f>
+        <v>7.1474700000000004E-7</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -7216,10 +7382,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D808FE82-F88E-9643-85A3-7681782C4413}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7273,10 +7439,10 @@
         <f t="shared" ref="E2:E3" si="1">C2*1.1</f>
         <v>4.0399497629947734E-3</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -7299,15 +7465,15 @@
         <f t="shared" si="1"/>
         <v>3.4724800000000003E-4</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -7324,15 +7490,15 @@
         <f t="shared" ref="E4:E15" si="3">C4*1.1</f>
         <v>2.7726600000000001</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -7349,7 +7515,7 @@
         <f t="shared" ref="E5" si="5">C5*1.1</f>
         <v>47.842300000000009</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -7374,10 +7540,10 @@
         <f t="shared" si="3"/>
         <v>1.3404600000000003E-2</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -7399,7 +7565,7 @@
         <f t="shared" si="3"/>
         <v>5.3025500000000005E-3</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -7424,7 +7590,7 @@
         <f t="shared" ref="E8" si="7">C8*1.1</f>
         <v>5.8356100000000006E-3</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -7449,7 +7615,7 @@
         <f t="shared" si="3"/>
         <v>9.7974800000000008E-3</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -7463,7 +7629,7 @@
       <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <f>0.00099355/20+19/20*C24</f>
         <v>5.0386599E-5</v>
       </c>
@@ -7475,7 +7641,7 @@
         <f t="shared" si="3"/>
         <v>5.5425258900000002E-5</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -7500,7 +7666,7 @@
         <f t="shared" si="3"/>
         <v>7.9536600000000013E-3</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -7525,7 +7691,7 @@
         <f t="shared" si="3"/>
         <v>5.7799499999999998E-3</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -7550,7 +7716,7 @@
         <f t="shared" si="3"/>
         <v>1.8850700000000002E-3</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -7575,7 +7741,7 @@
         <f t="shared" si="3"/>
         <v>3.7368100000000006E-3</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -7600,10 +7766,10 @@
         <f t="shared" si="3"/>
         <v>3.3018700000000002E-3</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -7626,7 +7792,7 @@
         <f t="shared" ref="E16:E17" si="9">C16*1.1</f>
         <v>-1.1484954056476917E-3</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -7651,7 +7817,7 @@
         <f t="shared" si="9"/>
         <v>-4.8970900000000006E-3</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -7665,7 +7831,7 @@
       <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="2">
         <f>C36*24.624</f>
         <v>9.7373145599999994E-4</v>
       </c>
@@ -7677,7 +7843,7 @@
         <f>C18*1.1</f>
         <v>1.0711046016000001E-3</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -7702,7 +7868,7 @@
         <f>C19*1.1</f>
         <v>1.6867400000000002E-3</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -7727,7 +7893,7 @@
         <f>C20*1.1</f>
         <v>-2.1401600000000003E-3</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -7753,7 +7919,7 @@
         <f>C21*1.1</f>
         <v>7.4089176163956241</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -7779,7 +7945,7 @@
         <f>C22*1.1</f>
         <v>3.2419214678217401E-2</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -7804,7 +7970,7 @@
         <f t="shared" ref="E23:E38" si="11">C23*1.1</f>
         <v>5.5385000000000009E-3</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -7818,7 +7984,7 @@
       <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="4">
         <v>7.4641999999999998E-7</v>
       </c>
       <c r="D24" s="2">
@@ -7829,7 +7995,7 @@
         <f t="shared" si="11"/>
         <v>8.2106200000000008E-7</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -7854,7 +8020,7 @@
         <f t="shared" si="11"/>
         <v>4.7399000000000009E-3</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -7879,7 +8045,7 @@
         <f t="shared" si="11"/>
         <v>0.124366</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -7904,7 +8070,7 @@
         <f t="shared" si="11"/>
         <v>8.9618100000000006E-2</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -7929,7 +8095,7 @@
         <f t="shared" si="11"/>
         <v>3.4514700000000002E-4</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -7954,7 +8120,7 @@
         <f t="shared" si="11"/>
         <v>5.7799499999999998E-3</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -7979,7 +8145,7 @@
         <f t="shared" si="11"/>
         <v>2.1401600000000003E-3</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -8004,7 +8170,7 @@
         <f t="shared" si="11"/>
         <v>8.3801299999999995E-3</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
@@ -8029,7 +8195,7 @@
         <f t="shared" si="11"/>
         <v>1258.0700000000002</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -8054,7 +8220,7 @@
         <f t="shared" si="11"/>
         <v>2.5962199999999998E-3</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -8079,7 +8245,7 @@
         <f t="shared" si="11"/>
         <v>1.0959960000000001E-3</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -8093,7 +8259,7 @@
       <c r="B35" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="4">
         <v>7.2872000000000003E-5</v>
       </c>
       <c r="D35" s="2">
@@ -8104,7 +8270,7 @@
         <f t="shared" si="11"/>
         <v>8.0159200000000003E-5</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -8118,7 +8284,7 @@
       <c r="B36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="4">
         <v>3.9544E-5</v>
       </c>
       <c r="D36" s="2">
@@ -8129,7 +8295,7 @@
         <f t="shared" si="11"/>
         <v>4.3498400000000004E-5</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -8154,7 +8320,7 @@
         <f t="shared" si="11"/>
         <v>1.7771600000000002E-4</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G37" s="2" t="s">
@@ -8179,10 +8345,35 @@
         <f t="shared" si="11"/>
         <v>1.6867400000000002E-3</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1.82E-3</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" ref="D39" si="12">C39*0.9</f>
+        <v>1.6380000000000001E-3</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" ref="E39" si="13">C39*1.1</f>
+        <v>2.0020000000000003E-3</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -8194,10 +8385,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A51A52-8F98-9E4F-A71B-2360CB867449}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8250,10 +8441,10 @@
         <f t="shared" ref="E2:E3" si="1">C2*1.1</f>
         <v>4.9424996961471457E-2</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -8276,15 +8467,15 @@
         <f t="shared" si="1"/>
         <v>2.4205720000000004E-4</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -8301,15 +8492,15 @@
         <f t="shared" ref="E4:E15" si="3">C4*1.1</f>
         <v>99.265100000000004</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -8326,7 +8517,7 @@
         <f t="shared" ref="E5" si="5">C5*1.1</f>
         <v>1497.43</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -8351,10 +8542,10 @@
         <f t="shared" si="3"/>
         <v>0.152394</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -8376,7 +8567,7 @@
         <f t="shared" si="3"/>
         <v>1.17678E-2</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -8401,7 +8592,7 @@
         <f t="shared" ref="E8" si="7">C8*1.1</f>
         <v>8.0436400000000012E-3</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -8426,7 +8617,7 @@
         <f t="shared" si="3"/>
         <v>3.8270100000000008E-2</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -8440,7 +8631,7 @@
       <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <f>0.03472/20+19/20*C24</f>
         <v>1.7418828750000001E-3</v>
       </c>
@@ -8452,7 +8643,7 @@
         <f t="shared" si="3"/>
         <v>1.9160711625000003E-3</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -8477,7 +8668,7 @@
         <f t="shared" si="3"/>
         <v>5.6031800000000001E-3</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -8502,7 +8693,7 @@
         <f t="shared" si="3"/>
         <v>2.8901399999999998E-3</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -8527,7 +8718,7 @@
         <f t="shared" si="3"/>
         <v>2.0467699999999998E-2</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -8552,7 +8743,7 @@
         <f t="shared" si="3"/>
         <v>7.704840000000001E-3</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -8577,10 +8768,10 @@
         <f t="shared" si="3"/>
         <v>1.1031900000000001E-2</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -8603,7 +8794,7 @@
         <f t="shared" ref="E16:E17" si="9">C16*1.1</f>
         <v>-3.28131969072165E-3</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -8628,7 +8819,7 @@
         <f t="shared" si="9"/>
         <v>-4.0416199999999999E-2</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -8642,7 +8833,7 @@
       <c r="B18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="2">
         <f>C36*24.624</f>
         <v>6.6642393600000003E-4</v>
       </c>
@@ -8654,7 +8845,7 @@
         <f>C18*1.1</f>
         <v>7.3306632960000006E-4</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -8679,7 +8870,7 @@
         <f>C19*1.1</f>
         <v>1.2370599999999999E-3</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -8704,7 +8895,7 @@
         <f>C20*1.1</f>
         <v>-7.6177199999999997E-4</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -8730,7 +8921,7 @@
         <f>C21*1.1</f>
         <v>1.7784502059432854</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -8756,7 +8947,7 @@
         <f>C22*1.1</f>
         <v>0.31611401185589505</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -8781,7 +8972,7 @@
         <f t="shared" ref="E23:E38" si="11">C23*1.1</f>
         <v>1.2280400000000002E-2</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -8795,7 +8986,7 @@
       <c r="B24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="4">
         <v>6.1924999999999996E-6</v>
       </c>
       <c r="D24" s="2">
@@ -8806,7 +8997,7 @@
         <f t="shared" si="11"/>
         <v>6.8117500000000005E-6</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -8831,7 +9022,7 @@
         <f t="shared" si="11"/>
         <v>6.9273600000000005E-2</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -8856,7 +9047,7 @@
         <f t="shared" si="11"/>
         <v>0.11379500000000001</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -8881,7 +9072,7 @@
         <f t="shared" si="11"/>
         <v>3.4271600000000007</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -8906,7 +9097,7 @@
         <f t="shared" si="11"/>
         <v>1.6669400000000003E-4</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -8931,7 +9122,7 @@
         <f t="shared" si="11"/>
         <v>2.8901399999999998E-3</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -8956,7 +9147,7 @@
         <f t="shared" si="11"/>
         <v>7.6177199999999997E-4</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -8981,7 +9172,7 @@
         <f t="shared" si="11"/>
         <v>9.120650000000001E-3</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
@@ -9006,7 +9197,7 @@
         <f t="shared" si="11"/>
         <v>300.83900000000006</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -9031,7 +9222,7 @@
         <f t="shared" si="11"/>
         <v>5.7019600000000007E-3</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -9056,7 +9247,7 @@
         <f t="shared" si="11"/>
         <v>7.7420199999999998E-4</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -9081,7 +9272,7 @@
         <f t="shared" si="11"/>
         <v>4.5994300000000004E-4</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -9095,7 +9286,7 @@
       <c r="B36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="4">
         <v>2.7064E-5</v>
       </c>
       <c r="D36" s="2">
@@ -9106,7 +9297,7 @@
         <f t="shared" si="11"/>
         <v>2.9770400000000002E-5</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -9131,7 +9322,7 @@
         <f t="shared" si="11"/>
         <v>1.3299000000000001E-4</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G37" s="2" t="s">
@@ -9156,10 +9347,35 @@
         <f t="shared" si="11"/>
         <v>1.2370599999999999E-3</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="2">
+        <v>5.3932000000000003E-4</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" ref="D39" si="12">C39*0.9</f>
+        <v>4.8538800000000006E-4</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" ref="E39" si="13">C39*1.1</f>
+        <v>5.9325200000000006E-4</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -9171,10 +9387,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{868E75BC-0D54-F046-9DC9-380953A4C8CF}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9227,10 +9443,10 @@
         <f t="shared" ref="E2:E3" si="1">C2*1.1</f>
         <v>54.540444840578537</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -9253,15 +9469,15 @@
         <f t="shared" si="1"/>
         <v>1.406328</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -9278,15 +9494,15 @@
         <f t="shared" ref="E4:E15" si="3">C4*1.1</f>
         <v>87151.900000000009</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -9303,7 +9519,7 @@
         <f t="shared" ref="E5" si="5">C5*1.1</f>
         <v>1337380</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -9328,10 +9544,10 @@
         <f t="shared" si="3"/>
         <v>181.203</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -9353,7 +9569,7 @@
         <f t="shared" si="3"/>
         <v>27.732099999999999</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -9378,7 +9594,7 @@
         <f t="shared" ref="E8" si="7">C8*1.1</f>
         <v>27.221700000000002</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -9403,7 +9619,7 @@
         <f t="shared" si="3"/>
         <v>34.980000000000004</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -9429,7 +9645,7 @@
         <f t="shared" si="3"/>
         <v>1.850615965</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -9454,7 +9670,7 @@
         <f t="shared" si="3"/>
         <v>9.5607600000000001</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -9479,7 +9695,7 @@
         <f t="shared" si="3"/>
         <v>9.4255700000000004</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -9504,7 +9720,7 @@
         <f t="shared" si="3"/>
         <v>507.69400000000007</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -9529,7 +9745,7 @@
         <f t="shared" si="3"/>
         <v>14.550800000000001</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -9554,10 +9770,10 @@
         <f t="shared" si="3"/>
         <v>16.335000000000001</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -9580,7 +9796,7 @@
         <f t="shared" ref="E16:E17" si="9">C16*1.1</f>
         <v>-4.9461868803227258</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -9605,7 +9821,7 @@
         <f t="shared" si="9"/>
         <v>-69.225200000000001</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -9619,7 +9835,7 @@
       <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="2">
         <f>C36*24.624</f>
         <v>3.6320399999999995</v>
       </c>
@@ -9631,7 +9847,7 @@
         <f>C18*1.1</f>
         <v>3.9952439999999996</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -9656,7 +9872,7 @@
         <f>C19*1.1</f>
         <v>2.3401400000000003</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -9681,7 +9897,7 @@
         <f>C20*1.1</f>
         <v>-3.2209100000000004</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -9707,7 +9923,7 @@
         <f>C21*1.1</f>
         <v>30036.958170812293</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -9733,7 +9949,7 @@
         <f>C22*1.1</f>
         <v>406.41361434068995</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -9758,7 +9974,7 @@
         <f t="shared" ref="E23:E38" si="11">C23*1.1</f>
         <v>15.804800000000002</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -9783,7 +9999,7 @@
         <f t="shared" si="11"/>
         <v>1.09747E-2</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -9808,7 +10024,7 @@
         <f t="shared" si="11"/>
         <v>67.622500000000002</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -9833,7 +10049,7 @@
         <f t="shared" si="11"/>
         <v>692.3180000000001</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -9858,7 +10074,7 @@
         <f t="shared" si="11"/>
         <v>3483.92</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -9883,7 +10099,7 @@
         <f t="shared" si="11"/>
         <v>1.3762100000000002</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -9908,7 +10124,7 @@
         <f t="shared" si="11"/>
         <v>9.4255700000000004</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -9933,7 +10149,7 @@
         <f t="shared" si="11"/>
         <v>3.2209100000000004</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -9958,7 +10174,7 @@
         <f t="shared" si="11"/>
         <v>19.179600000000001</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
@@ -9983,7 +10199,7 @@
         <f t="shared" si="11"/>
         <v>5102790</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -10008,7 +10224,7 @@
         <f t="shared" si="11"/>
         <v>9.2582600000000017</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -10033,7 +10249,7 @@
         <f t="shared" si="11"/>
         <v>1.6073200000000001</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -10058,7 +10274,7 @@
         <f t="shared" si="11"/>
         <v>0.50837600000000005</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -10083,7 +10299,7 @@
         <f t="shared" si="11"/>
         <v>0.16225000000000001</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -10108,7 +10324,7 @@
         <f t="shared" si="11"/>
         <v>0.33654500000000004</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G37" s="2" t="s">
@@ -10133,10 +10349,35 @@
         <f t="shared" si="11"/>
         <v>2.3401400000000003</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="2">
+        <v>2.2524000000000002</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" ref="D39" si="12">C39*0.9</f>
+        <v>2.0271600000000003</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" ref="E39" si="13">C39*1.1</f>
+        <v>2.4776400000000005</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
better characterize different feedstocks
</commit_message>
<xml_diff>
--- a/exposan/htl/data/impact_items.xlsx
+++ b/exposan/htl/data/impact_items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiananfeng/Desktop/PhD_CEE/coding/cloned_packages/EXPOsan/exposan/htl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6F0A10-2DD1-8240-AC06-808B31836331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0B4CA4-50CA-F74F-86ED-5E59081CF6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="11300" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="2400" yWindow="10240" windowWidth="50000" windowHeight="28300" activeTab="4" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -5623,7 +5623,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9757,11 +9757,11 @@
         <v>5.3932000000000003E-4</v>
       </c>
       <c r="D39" s="2">
-        <f t="shared" ref="D39:D40" si="12">C39*0.9</f>
+        <f t="shared" ref="D39" si="12">C39*0.9</f>
         <v>4.8538800000000006E-4</v>
       </c>
       <c r="E39" s="2">
-        <f t="shared" ref="E39:E40" si="13">C39*1.1</f>
+        <f t="shared" ref="E39" si="13">C39*1.1</f>
         <v>5.9325200000000006E-4</v>
       </c>
       <c r="F39" s="2" t="s">

</xml_diff>

<commit_message>
update geospatial system and analysis
</commit_message>
<xml_diff>
--- a/exposan/htl/data/impact_items.xlsx
+++ b/exposan/htl/data/impact_items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiananfeng/Desktop/PhD_CEE/coding/cloned_packages/EXPOsan/exposan/htl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0B4CA4-50CA-F74F-86ED-5E59081CF6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D684204E-D27D-304E-B661-E7969A74C3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="10240" windowWidth="50000" windowHeight="28300" activeTab="4" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="11600" yWindow="5200" windowWidth="28800" windowHeight="17500" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="115">
   <si>
     <t>ecoinvent 3</t>
   </si>
@@ -363,9 +363,6 @@
     <t>market for natural gas, burned in gas motor, for storage</t>
   </si>
   <si>
-    <t>includle burning emission, 1 kg natural gas = 24.624 MJ (see Ecoinvent: market for natural gas liquids)</t>
-  </si>
-  <si>
     <t>market for naphtha</t>
   </si>
   <si>
@@ -385,13 +382,29 @@
   </si>
   <si>
     <t>market for petroleum</t>
+  </si>
+  <si>
+    <t>heat and power co-generation, natural gas, mini-plant 2KW electrical</t>
+  </si>
+  <si>
+    <t>1 kg natural gas/CH4 = 54.2100427046263 MJ (arbitrary value, natural gas: 42-55 MJ/kg [source: https://world-nuclear.org/information-library/facts-and-figures/heat-values-of-various-fuels.aspx], CH4: 55.5 MJ/kg [source: BioSTEAM], note by comparing CHP of different size, we can see the size does not have a relationship with LCIA)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="8">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
+    <numFmt numFmtId="167" formatCode="0.000000000000"/>
+    <numFmt numFmtId="168" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="169" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="170" formatCode="_(* #,##0.0000000000_);_(* \(#,##0.0000000000\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -424,6 +437,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -442,20 +468,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -770,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66379A7A-E84B-1346-816F-577916F7D6A6}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,7 +818,7 @@
     <col min="2" max="2" width="18.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="201.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
@@ -1051,13 +1089,13 @@
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1098,11 +1136,11 @@
       <c r="B21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -1111,11 +1149,11 @@
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
@@ -1355,13 +1393,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>48</v>
@@ -1369,13 +1407,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>48</v>
@@ -1383,13 +1421,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>33</v>
@@ -1408,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32918E97-33AC-4743-867D-87B08CF8DB3F}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1857,16 +1895,15 @@
         <v>28</v>
       </c>
       <c r="C18" s="2">
-        <f>C36*24.624</f>
-        <v>3.50916624E-4</v>
+        <v>3.2652877122704623E-4</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>3.1582496160000002E-4</v>
+        <v>2.9387589410434159E-4</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>3.8600828640000004E-4</v>
+        <v>3.5918164834975087E-4</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>1</v>
@@ -2379,7 +2416,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>28</v>
@@ -2404,7 +2441,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>28</v>
@@ -2429,7 +2466,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>28</v>
@@ -2464,7 +2501,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2912,16 +2949,15 @@
         <v>21</v>
       </c>
       <c r="C18" s="2">
-        <f>C36*24.624</f>
-        <v>8.3822558399999997E-2</v>
+        <v>8.6654753263345194E-2</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>7.5440302560000005E-2</v>
+        <v>7.7989277937010673E-2</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>9.2204814240000002E-2</v>
+        <v>9.5320228589679715E-2</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>1</v>
@@ -3434,7 +3470,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>21</v>
@@ -3459,7 +3495,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>21</v>
@@ -3484,7 +3520,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>21</v>
@@ -3518,7 +3554,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3964,16 +4000,15 @@
         <v>22</v>
       </c>
       <c r="C18" s="2">
-        <f>C36*24.624</f>
-        <v>6.3446198400000001E-2</v>
+        <v>0.10460911940711742</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>5.7101578560000005E-2</v>
+        <v>9.4148207466405689E-2</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>6.979081824000001E-2</v>
+        <v>0.11507003134782917</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>1</v>
@@ -4486,7 +4521,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>22</v>
@@ -4511,7 +4546,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>22</v>
@@ -4536,7 +4571,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>22</v>
@@ -4569,8 +4604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CC6322-9D61-AD41-A8B1-E5A60BE6F0EB}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5017,16 +5052,15 @@
         <v>23</v>
       </c>
       <c r="C18" s="4">
-        <f>C36*24.624</f>
-        <v>7.2539841599999995E-5</v>
+        <v>7.5964532841992879E-5</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>6.5285857439999992E-5</v>
+        <v>6.8368079557793587E-5</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>7.9793825759999997E-5</v>
+        <v>8.3560986126192171E-5</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>1</v>
@@ -5539,7 +5573,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>23</v>
@@ -5564,7 +5598,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>23</v>
@@ -5589,7 +5623,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>23</v>
@@ -5620,10 +5654,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE2E960-887B-1E49-80AF-9619BDC224B9}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K24" sqref="K24:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5632,6 +5666,10 @@
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -6035,7 +6073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>96</v>
       </c>
@@ -6059,8 +6097,9 @@
       <c r="G17" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>97</v>
       </c>
@@ -6068,7 +6107,6 @@
         <v>11</v>
       </c>
       <c r="C18" s="2">
-        <f>C36*24.624</f>
         <v>1.584234288</v>
       </c>
       <c r="D18" s="2">
@@ -6085,8 +6123,11 @@
       <c r="G18" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J18" s="6"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>87</v>
       </c>
@@ -6110,8 +6151,9 @@
       <c r="G19" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>88</v>
       </c>
@@ -6135,8 +6177,10 @@
       <c r="G20" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J20" s="6"/>
+      <c r="N20" s="12"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>98</v>
       </c>
@@ -6161,8 +6205,9 @@
       <c r="G21" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>103</v>
       </c>
@@ -6187,8 +6232,9 @@
       <c r="G22" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>58</v>
       </c>
@@ -6213,7 +6259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>99</v>
       </c>
@@ -6238,7 +6284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>59</v>
       </c>
@@ -6263,7 +6309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>60</v>
       </c>
@@ -6287,8 +6333,9 @@
       <c r="G26" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K26" s="9"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>61</v>
       </c>
@@ -6313,7 +6360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
@@ -6338,7 +6385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>90</v>
       </c>
@@ -6363,7 +6410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>104</v>
       </c>
@@ -6387,8 +6434,9 @@
       <c r="G30" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N30" s="10"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>100</v>
       </c>
@@ -6412,8 +6460,9 @@
       <c r="G31" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N31" s="10"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>79</v>
       </c>
@@ -6437,8 +6486,9 @@
       <c r="G32" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N32" s="10"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>62</v>
       </c>
@@ -6462,8 +6512,9 @@
       <c r="G33" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="Q33" s="5"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>63</v>
       </c>
@@ -6488,7 +6539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>91</v>
       </c>
@@ -6512,8 +6563,9 @@
       <c r="G35" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="O35" s="11"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>101</v>
       </c>
@@ -6538,7 +6590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>92</v>
       </c>
@@ -6563,7 +6615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>102</v>
       </c>
@@ -6588,9 +6640,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>11</v>
@@ -6613,9 +6665,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>11</v>
@@ -6638,9 +6690,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>11</v>
@@ -6662,6 +6714,77 @@
       <c r="G41" s="2" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="N44" s="10"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="13"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="13"/>
+      <c r="R47" s="13"/>
+      <c r="S47" s="13"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="13"/>
+      <c r="P48" s="13"/>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="13"/>
+      <c r="S48" s="13"/>
+    </row>
+    <row r="50" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="13"/>
+      <c r="O50" s="13"/>
+      <c r="P50" s="13"/>
+      <c r="Q50" s="13"/>
+      <c r="R50" s="13"/>
+      <c r="S50" s="13"/>
+    </row>
+    <row r="52" spans="7:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="G52" s="6"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="14"/>
+      <c r="N52" s="14"/>
+      <c r="O52" s="14"/>
+      <c r="P52" s="14"/>
+      <c r="Q52" s="14"/>
+      <c r="R52" s="14"/>
+      <c r="S52" s="14"/>
+    </row>
+    <row r="55" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="N55" s="7"/>
+    </row>
+    <row r="56" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="N56" s="7"/>
+    </row>
+    <row r="57" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="N57" s="7"/>
+    </row>
+    <row r="58" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="N58" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -6673,8 +6796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578089A2-98D2-704F-AF44-C2497A6C7B0D}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7121,16 +7244,15 @@
         <v>24</v>
       </c>
       <c r="C18" s="2">
-        <f>C36*24.624</f>
-        <v>1.2338347679999998E-7</v>
+        <v>1.3692372586334518E-7</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>1.1104512911999998E-7</v>
+        <v>1.2323135327701067E-7</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>1.3572182447999999E-7</v>
+        <v>1.5061609844967972E-7</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>1</v>
@@ -7643,7 +7765,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>24</v>
@@ -7668,7 +7790,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>24</v>
@@ -7693,7 +7815,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>24</v>
@@ -7726,8 +7848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D808FE82-F88E-9643-85A3-7681782C4413}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8174,16 +8296,15 @@
         <v>25</v>
       </c>
       <c r="C18" s="2">
-        <f>C36*24.624</f>
-        <v>9.7373145599999994E-4</v>
+        <v>1.1151547884768684E-3</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>8.7635831040000002E-4</v>
+        <v>1.0036393096291816E-3</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>1.0711046016000001E-3</v>
+        <v>1.2266702673245553E-3</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>1</v>
@@ -8696,7 +8817,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>25</v>
@@ -8721,7 +8842,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>25</v>
@@ -8746,7 +8867,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>25</v>
@@ -8780,7 +8901,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9226,16 +9347,15 @@
         <v>26</v>
       </c>
       <c r="C18" s="2">
-        <f>C36*24.624</f>
-        <v>6.6642393600000003E-4</v>
+        <v>1.4452397385053379E-3</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>5.9978154239999999E-4</v>
+        <v>1.3007157646548041E-3</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>7.3306632960000006E-4</v>
+        <v>1.5897637123558719E-3</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>1</v>
@@ -9748,7 +9868,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>26</v>
@@ -9773,7 +9893,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>26</v>
@@ -9798,7 +9918,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>26</v>
@@ -9831,8 +9951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{868E75BC-0D54-F046-9DC9-380953A4C8CF}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10278,16 +10398,15 @@
         <v>27</v>
       </c>
       <c r="C18" s="2">
-        <f>C36*24.624</f>
-        <v>3.6320399999999995</v>
+        <v>3.5066850324341634</v>
       </c>
       <c r="D18" s="2">
         <f>C18*0.9</f>
-        <v>3.2688359999999994</v>
+        <v>3.1560165291907469</v>
       </c>
       <c r="E18" s="2">
         <f>C18*1.1</f>
-        <v>3.9952439999999996</v>
+        <v>3.8573535356775799</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>1</v>
@@ -10800,7 +10919,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>27</v>
@@ -10825,7 +10944,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>27</v>
@@ -10850,7 +10969,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>27</v>

</xml_diff>